<commit_message>
adjusting FME2019 --> FME2020 in batch file
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="84">
   <si>
     <t>Nom du transformer</t>
   </si>
@@ -35,14 +35,254 @@
     <t>Présent (Oui/Non)</t>
   </si>
   <si>
-    <t>Qui le prend?</t>
+    <t>AB_MISSING_ATTRIBUTE_MANAGER</t>
+  </si>
+  <si>
+    <t>AB_RESOURCES_FORMATTER</t>
+  </si>
+  <si>
+    <t>BC_DATA_READER</t>
+  </si>
+  <si>
+    <t>BC_GEOWAREHOUSE_URL_BUILDER</t>
+  </si>
+  <si>
+    <t>BC_RESOURCE_NAME_CORRECTION</t>
+  </si>
+  <si>
+    <t>BC_WMS_FORMATTER</t>
+  </si>
+  <si>
+    <t>DEFAULT_ATTRIBUTE_MAPPER</t>
+  </si>
+  <si>
+    <t>DUPLICATE_SERVICE_REMOVER</t>
+  </si>
+  <si>
+    <t>EMAIL_FORMAT_TESTER</t>
+  </si>
+  <si>
+    <t>FORMAT_VALIDATOR</t>
+  </si>
+  <si>
+    <t>GMD_SECTION_DATA_EXTRACTION</t>
+  </si>
+  <si>
+    <t>METADATA_FORMAT_MAPPER</t>
+  </si>
+  <si>
+    <t>METADATA_VALUE_MAPPER</t>
+  </si>
+  <si>
+    <t>MORE_INFO_MANAGER</t>
+  </si>
+  <si>
+    <t>ON_TRANSFER_LANG_MAPPER</t>
+  </si>
+  <si>
+    <t>QC_MISSING_EMAIL_SETTER</t>
+  </si>
+  <si>
+    <t>REMOVE_BROKEN_URL_WMS_ESRI_REST</t>
+  </si>
+  <si>
+    <t>RESOURCES_VALIDATOR</t>
+  </si>
+  <si>
+    <t>RESOURCE_NAME_UNDERSCORE_REMOVER</t>
+  </si>
+  <si>
+    <t>SOCRATA_RESOURCE_MAPPER</t>
+  </si>
+  <si>
+    <t>SocrataAPICaller</t>
+  </si>
+  <si>
+    <t>SocrataDateTimeConverter</t>
+  </si>
+  <si>
+    <t>SocrataHashIDGenerator</t>
+  </si>
+  <si>
+    <t>TEMPORAL_EXTENTS_MAPPER</t>
+  </si>
+  <si>
+    <t>TOPIC_PARSER</t>
+  </si>
+  <si>
+    <t>WMS_REST_LANGUAGE_FORMATTER</t>
+  </si>
+  <si>
+    <t>XML_PUBLISHER</t>
+  </si>
+  <si>
+    <t>AB_DATA_READER</t>
+  </si>
+  <si>
+    <t>AB_FGP_XML_BUILDER_PROD_05</t>
+  </si>
+  <si>
+    <t>AB_GEODISCOVER_RESOURCE_EXTRACTOR</t>
+  </si>
+  <si>
+    <t>AMPERSAND_CHARACTER_REFERENCE_REMOVER</t>
+  </si>
+  <si>
+    <t>ATTRIBUTE_VALUE_TEXT_CLEANER</t>
+  </si>
+  <si>
+    <t>AWS_TRANSLATE</t>
+  </si>
+  <si>
+    <t>BC_FGP_XML_BUILDER_PROD_04</t>
+  </si>
+  <si>
+    <t>EMPTY_FORMAT_MAPPER</t>
+  </si>
+  <si>
+    <t>GEOPORTAL_WEBLINK_ADDER</t>
+  </si>
+  <si>
+    <t>GEOSPATIAL_DATA_VALIDATOR</t>
+  </si>
+  <si>
+    <t>GEO_EXTENTS_MAPPER</t>
+  </si>
+  <si>
+    <t>JSON_PUBLISHER</t>
+  </si>
+  <si>
+    <t>LICENSE_FILTER</t>
+  </si>
+  <si>
+    <t>LOOKUP_TABLES_READER</t>
+  </si>
+  <si>
+    <t>MANUAL_GEOSPATIAL_SETTER</t>
+  </si>
+  <si>
+    <t>MAP_RESOURCE_ATTRIBUTION_REMOVER</t>
+  </si>
+  <si>
+    <t>METADATA_DELTA_FINDER</t>
+  </si>
+  <si>
+    <t>METADATA_VALUE_MAPPER_ERROR_MANAGER</t>
+  </si>
+  <si>
+    <t>METADATA_VALUE_MAPPER_Nic</t>
+  </si>
+  <si>
+    <t>METADATA_VALUE_MAPPER_ONE2MANY</t>
+  </si>
+  <si>
+    <t>NB_BoundingBoxExtractor</t>
+  </si>
+  <si>
+    <t>NB_ESRIMAPPER</t>
+  </si>
+  <si>
+    <t>NB_FRENCH_TAG_SEPARATOR</t>
+  </si>
+  <si>
+    <t>NB_FrenchEnglishTitleDescSeparator</t>
+  </si>
+  <si>
+    <t>NB_ISOTOPIC_ASSIGNER</t>
+  </si>
+  <si>
+    <t>NB_ORGANIZATION_MAPPER</t>
+  </si>
+  <si>
+    <t>ON_DATA_READER</t>
+  </si>
+  <si>
+    <t>ON_DATE_FORMATTER</t>
+  </si>
+  <si>
+    <t>ON_GEOHUB_RESOURCE_EXTRACTOR</t>
+  </si>
+  <si>
+    <t>ON_KEYWORD_RENAMER</t>
+  </si>
+  <si>
+    <t>PYCSW_URL_MAPPER</t>
+  </si>
+  <si>
+    <t>QC_ATTRIBUTE_MAPPER</t>
+  </si>
+  <si>
+    <t>QC_DATA_READER</t>
+  </si>
+  <si>
+    <t>QC_DATE_FORMATTER</t>
+  </si>
+  <si>
+    <t>QC_PROJECTION_GEOEXTENTS_EXTRACTOR</t>
+  </si>
+  <si>
+    <t>QC_SECTOR_MAPPER_AND_FILTER</t>
+  </si>
+  <si>
+    <t>QC_TBS_ATTRIBUTE_VALUE_MAPPER</t>
+  </si>
+  <si>
+    <t>QC_WMS_URL_SETTER</t>
+  </si>
+  <si>
+    <t>SPATIAL_TYPE_MAPPER</t>
+  </si>
+  <si>
+    <t>TBS_DEFAULT_KEYWORD_TOPIC_SUBJECT</t>
+  </si>
+  <si>
+    <t>UNIQUE_ID_CREATOR</t>
+  </si>
+  <si>
+    <t>UPDATE_TO_PROGRESS_MAPPER</t>
+  </si>
+  <si>
+    <t>URL_CHARACTER_ENCODER</t>
+  </si>
+  <si>
+    <t>URL_HTTPS_MAKER</t>
+  </si>
+  <si>
+    <t>UUID_4_FORMATTER</t>
+  </si>
+  <si>
+    <t>YT_CATALOGUE_READER</t>
+  </si>
+  <si>
+    <t>YT_CONTACTS_MERGER</t>
+  </si>
+  <si>
+    <t>YT_DATA_READER</t>
+  </si>
+  <si>
+    <t>YT_DATE_FORMATTER</t>
+  </si>
+  <si>
+    <t>YT_GEOWEB_EXTRACTOR</t>
+  </si>
+  <si>
+    <t>YT_MISSING_ATTRIBUTE_MANAGER</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Qui le prend? (BCG/DP)</t>
+  </si>
+  <si>
+    <t>Non</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,13 +290,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9D1D9"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,13 +345,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -353,18 +656,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -374,14 +678,1116 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+    </row>
+    <row r="106" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+    </row>
+    <row r="121" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="2"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+    </row>
+    <row r="127" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="2"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+    </row>
+    <row r="133" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="2"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+    </row>
+    <row r="142" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+    </row>
+    <row r="148" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A151" s="2"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="2"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A157" s="2"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A160" s="2"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A163" s="2"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A166" s="2"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A169" s="2"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A172" s="2"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A175" s="2"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A178" s="2"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A181" s="2"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A184" s="2"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A187" s="2"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="190" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A190" s="2"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1"/>
+    </row>
+    <row r="193" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A193" s="2"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A196" s="2"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="199" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A199" s="2"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1"/>
+    </row>
+    <row r="202" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A202" s="2"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A205" s="2"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A208" s="2"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1"/>
+    </row>
+    <row r="211" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A211" s="2"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1"/>
+    </row>
+    <row r="214" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A214" s="2"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="217" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A217" s="2"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="1"/>
+    </row>
+    <row r="220" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A220" s="2"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="1"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1"/>
+    </row>
+    <row r="223" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A223" s="2"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1"/>
+    </row>
+    <row r="226" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A226" s="2"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="1"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A229" s="2"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1"/>
+    </row>
+    <row r="232" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A232" s="2"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A235" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New unit test for GEO_NONE_GEO_SELECTOR
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcrepeau\Documents\GitHub\fgp-metadata-proxy\FME_files\UNIT_TESTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FGP_GITHUB\fgp-metadata-proxy\FME_files\UNIT_TESTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$235</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$237</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="113">
   <si>
     <t>AB_MISSING_ATTRIBUTE_MANAGER</t>
   </si>
@@ -345,13 +345,34 @@
   </si>
   <si>
     <t>Benoît</t>
+  </si>
+  <si>
+    <t>LOOKUP_TABLES_READER_NG</t>
+  </si>
+  <si>
+    <t>Remplacer par LOOKUP_TABLES_READER_NG</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Remplace LOOKUP_TABLES_READER</t>
+  </si>
+  <si>
+    <t>Remplacer par GEO_NONE_GEO_SELECTOR</t>
+  </si>
+  <si>
+    <t>GEO_NONE_GEO_SELECTOR</t>
+  </si>
+  <si>
+    <t>Remplace GEO_NONE_GEO_SELECTOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,8 +494,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,6 +532,11 @@
       <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -595,11 +635,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -756,9 +797,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -775,7 +836,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1038,13 +1099,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H235"/>
+  <dimension ref="A1:H237"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
@@ -1502,53 +1563,59 @@
       <c r="G21" s="50"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:8" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" s="50"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="B22" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="61"/>
+      <c r="H22" s="63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" s="58" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="50"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>78</v>
@@ -1568,9 +1635,9 @@
       <c r="G24" s="50"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>42</v>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>78</v>
@@ -1590,9 +1657,9 @@
       <c r="G25" s="50"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>43</v>
+    <row r="26" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>78</v>
@@ -1614,7 +1681,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>78</v>
@@ -1636,7 +1703,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>78</v>
@@ -1656,123 +1723,123 @@
       <c r="G28" s="50"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="50"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="52"/>
-      <c r="H29" s="27" t="s">
+      <c r="B30" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="52"/>
+      <c r="H30" s="27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+    <row r="31" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="52"/>
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="B31" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="52"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G31" s="50"/>
-      <c r="H31" s="28" t="s">
+      <c r="B32" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="50"/>
+      <c r="H32" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G32" s="50"/>
-      <c r="H32" s="8"/>
-    </row>
-    <row r="33" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="B33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="50"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
         <v>51</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F33" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G33" s="52"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>78</v>
@@ -1793,30 +1860,30 @@
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="52"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" s="50"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>78</v>
@@ -1836,64 +1903,64 @@
       <c r="G36" s="50"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:8" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" s="50"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="B38" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="26"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" s="50"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="E39" s="22" t="s">
+      <c r="B39" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>79</v>
       </c>
       <c r="F39" s="34" t="s">
@@ -1902,32 +1969,32 @@
       <c r="G39" s="50"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="50"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="1:8" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" s="26"/>
-      <c r="H40" s="8"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="B41" s="5" t="s">
         <v>78</v>
       </c>
@@ -1940,15 +2007,15 @@
       <c r="E41" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G41" s="50"/>
+      <c r="F41" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="26"/>
       <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>78</v>
@@ -1968,9 +2035,9 @@
       <c r="G42" s="50"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>64</v>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>78</v>
@@ -1990,99 +2057,99 @@
       <c r="G43" s="50"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G44" s="50"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F44" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G44" s="26"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="B45" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="26"/>
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G45" s="50"/>
-      <c r="H45" s="8"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="B46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="50"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G46" s="52"/>
-      <c r="H46" s="28" t="s">
+      <c r="B47" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="52"/>
+      <c r="H47" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+    <row r="48" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F47" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G47" s="50"/>
-      <c r="H47" s="8"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>78</v>
@@ -2102,9 +2169,9 @@
       <c r="G48" s="50"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>67</v>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>78</v>
@@ -2124,9 +2191,9 @@
       <c r="G49" s="50"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>69</v>
+    <row r="50" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>78</v>
@@ -2146,9 +2213,9 @@
       <c r="G50" s="50"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>70</v>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>78</v>
@@ -2162,15 +2229,15 @@
       <c r="E51" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F51" s="36" t="s">
-        <v>102</v>
+      <c r="F51" s="34" t="s">
+        <v>79</v>
       </c>
       <c r="G51" s="50"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>25</v>
+    <row r="52" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>78</v>
@@ -2184,177 +2251,177 @@
       <c r="E52" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F52" s="34" t="s">
-        <v>79</v>
+      <c r="F52" s="36" t="s">
+        <v>102</v>
       </c>
       <c r="G52" s="50"/>
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G53" s="50"/>
+      <c r="H53" s="8"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F53" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G53" s="50"/>
-      <c r="H53" s="28" t="s">
+      <c r="B54" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G54" s="50"/>
+      <c r="H54" s="28" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F54" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G54" s="51" t="s">
+      <c r="B55" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="H54" s="8"/>
-    </row>
-    <row r="55" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+      <c r="H55" s="8"/>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F55" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G55" s="50"/>
-      <c r="H55" s="8"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="B56" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" s="50"/>
+      <c r="H56" s="8"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F56" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G56" s="51" t="s">
+      <c r="B57" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F57" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="H56" s="8"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="H57" s="8"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F57" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G57" s="50"/>
-      <c r="H57" s="8"/>
-    </row>
-    <row r="58" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="B58" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" s="50"/>
+      <c r="H58" s="8"/>
+    </row>
+    <row r="59" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F58" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G58" s="51" t="s">
+      <c r="B59" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G59" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="H58" s="8"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F59" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G59" s="50"/>
       <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>78</v>
@@ -2376,7 +2443,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>78</v>
@@ -2398,7 +2465,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>78</v>
@@ -2412,15 +2479,15 @@
       <c r="E62" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F62" s="36" t="s">
-        <v>102</v>
+      <c r="F62" s="34" t="s">
+        <v>79</v>
       </c>
       <c r="G62" s="50"/>
       <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>78</v>
@@ -2434,38 +2501,38 @@
       <c r="E63" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F63" s="34" t="s">
-        <v>79</v>
+      <c r="F63" s="36" t="s">
+        <v>102</v>
       </c>
       <c r="G63" s="50"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F64" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G64" s="50"/>
+      <c r="H64" s="8"/>
+    </row>
+    <row r="65" spans="1:8" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F64" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G64" s="26"/>
-      <c r="H64" s="8"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="B65" s="5" t="s">
         <v>78</v>
       </c>
@@ -2478,15 +2545,15 @@
       <c r="E65" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F65" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G65" s="50"/>
+      <c r="F65" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G65" s="26"/>
       <c r="H65" s="8"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>78</v>
@@ -2508,7 +2575,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>78</v>
@@ -2528,9 +2595,9 @@
       <c r="G67" s="50"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
-        <v>9</v>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>78</v>
@@ -2552,7 +2619,7 @@
     </row>
     <row r="69" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>78</v>
@@ -2572,9 +2639,9 @@
       <c r="G69" s="50"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>10</v>
+    <row r="70" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>78</v>
@@ -2596,7 +2663,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>78</v>
@@ -2618,7 +2685,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>78</v>
@@ -2638,31 +2705,33 @@
       <c r="G72" s="50"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F73" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G73" s="50"/>
-      <c r="H73" s="8"/>
+    <row r="73" spans="1:8" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="B73" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="E73" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="F73" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="G73" s="61"/>
+      <c r="H73" s="63" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>78</v>
@@ -2679,12 +2748,16 @@
       <c r="F74" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="G74" s="50"/>
-      <c r="H74" s="8"/>
+      <c r="G74" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="75" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>78</v>
@@ -2706,7 +2779,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>78</v>
@@ -2726,9 +2799,9 @@
       <c r="G76" s="50"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>56</v>
+    <row r="77" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>78</v>
@@ -2750,7 +2823,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>78</v>
@@ -2770,9 +2843,9 @@
       <c r="G78" s="50"/>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="10" t="s">
-        <v>59</v>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>78</v>
@@ -2792,31 +2865,31 @@
       <c r="G79" s="50"/>
       <c r="H79" s="8"/>
     </row>
-    <row r="80" spans="1:8" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B80" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="C80" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D80" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="E80" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="F80" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="G80" s="53"/>
-      <c r="H80" s="49"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>15</v>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F80" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G80" s="50"/>
+      <c r="H80" s="8"/>
+    </row>
+    <row r="81" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>78</v>
@@ -2836,31 +2909,31 @@
       <c r="G81" s="50"/>
       <c r="H81" s="8"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F82" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G82" s="50"/>
-      <c r="H82" s="8"/>
-    </row>
-    <row r="83" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
-        <v>18</v>
+    <row r="82" spans="1:8" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B82" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C82" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D82" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="E82" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F82" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="G82" s="53"/>
+      <c r="H82" s="49"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>78</v>
@@ -2882,7 +2955,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>78</v>
@@ -2896,107 +2969,107 @@
       <c r="E84" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F84" s="36" t="s">
-        <v>103</v>
+      <c r="F84" s="34" t="s">
+        <v>79</v>
       </c>
       <c r="G84" s="50"/>
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="24" t="s">
+      <c r="A85" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F85" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G85" s="50"/>
+      <c r="H85" s="8"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F86" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="G86" s="50"/>
+      <c r="H86" s="8"/>
+    </row>
+    <row r="87" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B85" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C85" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E85" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="F85" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G85" s="52"/>
-      <c r="H85" s="27" t="s">
+      <c r="B87" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E87" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F87" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G87" s="52"/>
+      <c r="H87" s="27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
+    <row r="88" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B86" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C86" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D86" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E86" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="F86" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G86" s="52"/>
-      <c r="H86" s="27" t="s">
+      <c r="B88" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E88" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F88" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G88" s="52"/>
+      <c r="H88" s="27" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D87" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F87" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G87" s="50"/>
-      <c r="H87" s="8"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F88" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G88" s="50"/>
-      <c r="H88" s="8"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>78</v>
@@ -3016,9 +3089,9 @@
       <c r="G89" s="50"/>
       <c r="H89" s="8"/>
     </row>
-    <row r="90" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
-        <v>26</v>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>78</v>
@@ -3038,596 +3111,640 @@
       <c r="G90" s="50"/>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="40" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F91" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G91" s="50"/>
+      <c r="H91" s="8"/>
+    </row>
+    <row r="92" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F92" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G92" s="50"/>
+      <c r="H92" s="8"/>
+    </row>
+    <row r="93" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="B91" s="42"/>
-      <c r="C91" s="42"/>
-      <c r="D91" s="42"/>
-      <c r="E91" s="42"/>
-      <c r="F91" s="42"/>
-      <c r="G91" s="54"/>
-      <c r="H91" s="48"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
+      <c r="B93" s="42"/>
+      <c r="C93" s="42"/>
+      <c r="D93" s="42"/>
+      <c r="E93" s="42"/>
+      <c r="F93" s="42"/>
+      <c r="G93" s="54"/>
+      <c r="H93" s="48"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
+    <row r="96" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
+    <row r="99" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
+    <row r="102" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
+    <row r="105" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
+    <row r="108" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
+    <row r="111" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
+    <row r="114" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="2"/>
-      <c r="B118" s="2"/>
+    <row r="117" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
+    <row r="120" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
+    <row r="123" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
+    <row r="126" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
+    <row r="129" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
-    </row>
-    <row r="133" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
+    <row r="132" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
-    </row>
-    <row r="136" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
+    <row r="135" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
-    </row>
-    <row r="139" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
+    <row r="138" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
-      <c r="B141" s="1"/>
-    </row>
-    <row r="142" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
+    <row r="141" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
-    </row>
-    <row r="145" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
+    <row r="144" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+      <c r="B144" s="2"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
-    </row>
-    <row r="148" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
+    <row r="147" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
-    </row>
-    <row r="151" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
+    <row r="150" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
-    </row>
-    <row r="154" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A154" s="2"/>
-      <c r="B154" s="2"/>
+    <row r="153" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
-    </row>
-    <row r="157" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A157" s="2"/>
-      <c r="B157" s="2"/>
+    <row r="156" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="2"/>
+      <c r="B156" s="2"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
-    </row>
-    <row r="160" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A160" s="2"/>
-      <c r="B160" s="2"/>
+    <row r="159" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A159" s="2"/>
+      <c r="B159" s="2"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
-    </row>
-    <row r="163" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A163" s="2"/>
-      <c r="B163" s="2"/>
+    <row r="162" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A162" s="2"/>
+      <c r="B162" s="2"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
-    </row>
-    <row r="166" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A166" s="2"/>
-      <c r="B166" s="2"/>
+    <row r="165" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A165" s="2"/>
+      <c r="B165" s="2"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
-    </row>
-    <row r="169" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A169" s="2"/>
-      <c r="B169" s="2"/>
+    <row r="168" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A168" s="2"/>
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
-    </row>
-    <row r="172" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A172" s="2"/>
-      <c r="B172" s="2"/>
+    <row r="171" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2"/>
+      <c r="B171" s="2"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
-    </row>
-    <row r="175" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A175" s="2"/>
-      <c r="B175" s="2"/>
+    <row r="174" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
+      <c r="B174" s="2"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
-    </row>
-    <row r="178" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A178" s="2"/>
-      <c r="B178" s="2"/>
+    <row r="177" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A177" s="2"/>
+      <c r="B177" s="2"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
-    </row>
-    <row r="181" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A181" s="2"/>
-      <c r="B181" s="2"/>
+    <row r="180" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A180" s="2"/>
+      <c r="B180" s="2"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="1"/>
-      <c r="B183" s="1"/>
-    </row>
-    <row r="184" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A184" s="2"/>
-      <c r="B184" s="2"/>
+    <row r="183" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A183" s="2"/>
+      <c r="B183" s="2"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-      <c r="B186" s="1"/>
-    </row>
-    <row r="187" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A187" s="2"/>
-      <c r="B187" s="2"/>
+    <row r="186" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A186" s="2"/>
+      <c r="B186" s="2"/>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
-    </row>
-    <row r="190" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A190" s="2"/>
-      <c r="B190" s="2"/>
+    <row r="189" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A189" s="2"/>
+      <c r="B189" s="2"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
-      <c r="B192" s="1"/>
-    </row>
-    <row r="193" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A193" s="2"/>
-      <c r="B193" s="2"/>
+    <row r="192" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A192" s="2"/>
+      <c r="B192" s="2"/>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
-      <c r="B195" s="1"/>
-    </row>
-    <row r="196" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A196" s="2"/>
-      <c r="B196" s="2"/>
+    <row r="195" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A195" s="2"/>
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="1"/>
-      <c r="B198" s="1"/>
-    </row>
-    <row r="199" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A199" s="2"/>
-      <c r="B199" s="2"/>
+    <row r="198" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A198" s="2"/>
+      <c r="B198" s="2"/>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="1"/>
-      <c r="B201" s="1"/>
-    </row>
-    <row r="202" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2"/>
+    <row r="201" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A201" s="2"/>
+      <c r="B201" s="2"/>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="1"/>
+      <c r="B202" s="1"/>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="1"/>
-      <c r="B204" s="1"/>
-    </row>
-    <row r="205" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A205" s="2"/>
-      <c r="B205" s="2"/>
+    <row r="204" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A204" s="2"/>
+      <c r="B204" s="2"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="1"/>
-      <c r="B207" s="1"/>
-    </row>
-    <row r="208" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A208" s="2"/>
-      <c r="B208" s="2"/>
+    <row r="207" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A207" s="2"/>
+      <c r="B207" s="2"/>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="1"/>
+      <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
-    </row>
-    <row r="211" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A211" s="2"/>
-      <c r="B211" s="2"/>
+    <row r="210" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A210" s="2"/>
+      <c r="B210" s="2"/>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="1"/>
+      <c r="B211" s="1"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="1"/>
-      <c r="B213" s="1"/>
-    </row>
-    <row r="214" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A214" s="2"/>
-      <c r="B214" s="2"/>
+    <row r="213" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A213" s="2"/>
+      <c r="B213" s="2"/>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="1"/>
+      <c r="B214" s="1"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="1"/>
-      <c r="B216" s="1"/>
-    </row>
-    <row r="217" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A217" s="2"/>
-      <c r="B217" s="2"/>
+    <row r="216" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A216" s="2"/>
+      <c r="B216" s="2"/>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="1"/>
-      <c r="B219" s="1"/>
-    </row>
-    <row r="220" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A220" s="2"/>
-      <c r="B220" s="2"/>
+    <row r="219" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A219" s="2"/>
+      <c r="B219" s="2"/>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="1"/>
-      <c r="B222" s="1"/>
-    </row>
-    <row r="223" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A223" s="2"/>
-      <c r="B223" s="2"/>
+    <row r="222" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A222" s="2"/>
+      <c r="B222" s="2"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="1"/>
-      <c r="B225" s="1"/>
-    </row>
-    <row r="226" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A226" s="2"/>
-      <c r="B226" s="2"/>
+    <row r="225" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A225" s="2"/>
+      <c r="B225" s="2"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="1"/>
+      <c r="B226" s="1"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="1"/>
-      <c r="B228" s="1"/>
-    </row>
-    <row r="229" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A229" s="2"/>
-      <c r="B229" s="2"/>
+    <row r="228" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A228" s="2"/>
+      <c r="B228" s="2"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="1"/>
+      <c r="B229" s="1"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="1"/>
-      <c r="B231" s="1"/>
-    </row>
-    <row r="232" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A232" s="2"/>
-      <c r="B232" s="2"/>
+    <row r="231" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A231" s="2"/>
+      <c r="B231" s="2"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="1"/>
+      <c r="B232" s="1"/>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="1"/>
-      <c r="B234" s="1"/>
-    </row>
-    <row r="235" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A235" s="2"/>
-      <c r="B235" s="2"/>
+    <row r="234" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A234" s="2"/>
+      <c r="B234" s="2"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="1"/>
+      <c r="B235" s="1"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="1"/>
+      <c r="B236" s="1"/>
+    </row>
+    <row r="237" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A237" s="2"/>
+      <c r="B237" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H235">
+  <autoFilter ref="A1:H237">
     <filterColumn colId="3">
       <filters blank="1">
         <filter val="unitaire"/>

</xml_diff>

<commit_message>
Récupération des fichiers du revert
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcrepeau\Documents\GitHub\fgp-metadata-proxy\FME_files\UNIT_TESTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FGP_GITHUB\fgp-metadata-proxy\FME_files\UNIT_TESTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -828,8 +828,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -846,7 +846,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1111,11 +1111,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Feedback et mise à jour des Tests
Revision et mise à jour de deux derniers Test Unitaires:
- URL_HTTPS_Maker -- Fixed les differences de may/min et https/http.
- URL_Character_encoder -- Ajout d'un deuxième test pour confirmer que la transformation des caractères '{' , '}' avec des '%7B' et '%7D' ne fonctionne pas.
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="133">
   <si>
     <t>AB_MISSING_ATTRIBUTE_MANAGER</t>
   </si>
@@ -400,9 +400,6 @@
     <t>Obsolète</t>
   </si>
   <si>
-    <t>Révisé par</t>
-  </si>
-  <si>
     <t>Inexistent Attribute in 'etalon' files
   --  xlsx_type:xlsx_none</t>
   </si>
@@ -422,7 +419,16 @@
     <t>Les codes de replacement '%7B et %7D ne se font pas convertir en charactères souhaités. À la place, Ils restent literales: '%7B' et '%7D' dans le string.</t>
   </si>
   <si>
-    <t>Resources{}.url avec des mayuscules/minuscules mismatchs</t>
+    <t>Resources{}.url avec des mayuscules/minuscules mismatchs; https/http mismatch</t>
+  </si>
+  <si>
+    <t>Benoît / David</t>
+  </si>
+  <si>
+    <t>david</t>
+  </si>
+  <si>
+    <t>Daniel / David</t>
   </si>
 </sst>
 </file>
@@ -1204,10 +1210,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:XEZ240"/>
+  <dimension ref="A1:XEY240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="103" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="103" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,10 +1227,9 @@
     <col min="7" max="7" width="20.5703125" style="54" customWidth="1"/>
     <col min="8" max="8" width="44.42578125" customWidth="1"/>
     <col min="9" max="9" width="38.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>101</v>
       </c>
@@ -1252,11 +1257,8 @@
       <c r="I1" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>80</v>
       </c>
@@ -1276,7 +1278,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>81</v>
       </c>
@@ -1296,7 +1298,7 @@
       <c r="G3" s="30"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
@@ -1316,7 +1318,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>83</v>
       </c>
@@ -1336,7 +1338,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>84</v>
       </c>
@@ -1356,7 +1358,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>85</v>
       </c>
@@ -1376,7 +1378,7 @@
       <c r="G7" s="30"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>86</v>
       </c>
@@ -1396,7 +1398,7 @@
       <c r="G8" s="30"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>87</v>
       </c>
@@ -1416,7 +1418,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -1436,7 +1438,7 @@
       <c r="G10" s="30"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>89</v>
       </c>
@@ -1456,7 +1458,7 @@
       <c r="G11" s="30"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>90</v>
       </c>
@@ -1476,7 +1478,7 @@
       <c r="G12" s="30"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1498,7 +1500,7 @@
       <c r="G13" s="30"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
@@ -1520,7 +1522,7 @@
       <c r="G14" s="30"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>30</v>
       </c>
@@ -1545,7 +1547,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
@@ -1565,15 +1567,12 @@
         <v>79</v>
       </c>
       <c r="G16" s="49" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="J16" t="s">
-        <v>118</v>
-      </c>
-      <c r="K16" s="63"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J16" s="63"/>
+    </row>
+    <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>2</v>
       </c>
@@ -1595,7 +1594,7 @@
       <c r="G17" s="49"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
@@ -1617,7 +1616,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1636,17 +1635,16 @@
       <c r="F19" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="49"/>
+      <c r="G19" s="49" t="s">
+        <v>131</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="J19" t="s">
-        <v>118</v>
-      </c>
-      <c r="K19" s="67"/>
-    </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="J19" s="67"/>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -1656,11 +1654,11 @@
       <c r="G20" s="49"/>
       <c r="H20" s="8"/>
       <c r="I20" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="K20" s="67"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="J20" s="67"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1679,14 +1677,13 @@
       <c r="F21" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="49"/>
+      <c r="G21" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H21" s="8"/>
-      <c r="J21" t="s">
-        <v>118</v>
-      </c>
-      <c r="K21" s="63"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="63"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1708,7 +1705,7 @@
       <c r="G22" s="49"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>36</v>
       </c>
@@ -1735,7 +1732,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>111</v>
       </c>
@@ -1755,16 +1752,13 @@
         <v>79</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="H24" s="56"/>
       <c r="I24" s="60"/>
-      <c r="J24" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="K24" s="65"/>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J24" s="65"/>
+    </row>
+    <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>39</v>
       </c>
@@ -1783,14 +1777,13 @@
       <c r="F25" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="49"/>
+      <c r="G25" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H25" s="8"/>
-      <c r="J25" t="s">
-        <v>118</v>
-      </c>
-      <c r="K25" s="63"/>
-    </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="J25" s="63"/>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
@@ -1809,17 +1802,16 @@
       <c r="F26" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="61"/>
+      <c r="G26" s="61" t="s">
+        <v>118</v>
+      </c>
       <c r="H26" s="8"/>
       <c r="I26" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="J26" t="s">
-        <v>118</v>
-      </c>
-      <c r="K26" s="63"/>
-    </row>
-    <row r="27" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J26" s="63"/>
+    </row>
+    <row r="27" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>42</v>
       </c>
@@ -1838,14 +1830,13 @@
       <c r="F27" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="49"/>
+      <c r="G27" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H27" s="8"/>
-      <c r="J27" t="s">
-        <v>118</v>
-      </c>
-      <c r="K27" s="66"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="66"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
@@ -1864,16 +1855,15 @@
       <c r="F28" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G28" s="49"/>
+      <c r="G28" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H28" s="8"/>
       <c r="I28" t="s">
-        <v>128</v>
-      </c>
-      <c r="J28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
@@ -1892,14 +1882,13 @@
       <c r="F29" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="49"/>
+      <c r="G29" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H29" s="8"/>
-      <c r="J29" t="s">
-        <v>118</v>
-      </c>
-      <c r="K29" s="66"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="66"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>44</v>
       </c>
@@ -1918,14 +1907,13 @@
       <c r="F30" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G30" s="49"/>
+      <c r="G30" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H30" s="8"/>
-      <c r="J30" t="s">
-        <v>118</v>
-      </c>
-      <c r="K30" s="66"/>
-    </row>
-    <row r="31" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="J30" s="66"/>
+    </row>
+    <row r="31" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>47</v>
       </c>
@@ -1952,7 +1940,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>48</v>
       </c>
@@ -1974,7 +1962,7 @@
       <c r="G32" s="51"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>49</v>
       </c>
@@ -2001,7 +1989,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>50</v>
       </c>
@@ -2028,7 +2016,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>114</v>
       </c>
@@ -2054,7 +2042,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>51</v>
       </c>
@@ -2076,7 +2064,7 @@
       <c r="G36" s="51"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>52</v>
       </c>
@@ -2098,7 +2086,7 @@
       <c r="G37" s="51"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
@@ -2120,7 +2108,7 @@
       <c r="G38" s="49"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:11" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>54</v>
       </c>
@@ -2142,7 +2130,7 @@
       <c r="G39" s="49"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>55</v>
       </c>
@@ -2164,7 +2152,7 @@
       <c r="G40" s="25"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>14</v>
       </c>
@@ -2186,7 +2174,7 @@
       <c r="G41" s="49"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>57</v>
       </c>
@@ -2208,7 +2196,7 @@
       <c r="G42" s="49"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>61</v>
       </c>
@@ -2230,7 +2218,7 @@
       <c r="G43" s="25"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>62</v>
       </c>
@@ -2252,7 +2240,7 @@
       <c r="G44" s="49"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
@@ -2274,7 +2262,7 @@
       <c r="G45" s="49"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>64</v>
       </c>
@@ -2296,7 +2284,7 @@
       <c r="G46" s="49"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>16</v>
       </c>
@@ -2318,7 +2306,7 @@
       <c r="G47" s="25"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>65</v>
       </c>
@@ -2337,17 +2325,16 @@
       <c r="F48" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="49"/>
+      <c r="G48" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H48" s="8"/>
       <c r="I48" s="62" t="s">
-        <v>124</v>
-      </c>
-      <c r="J48" t="s">
-        <v>118</v>
-      </c>
-      <c r="K48" s="67"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="J48" s="67"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>21</v>
       </c>
@@ -2374,7 +2361,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>66</v>
       </c>
@@ -2396,7 +2383,7 @@
       <c r="G50" s="49"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -2418,7 +2405,7 @@
       <c r="G51" s="49"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:11" s="22" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="22" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>67</v>
       </c>
@@ -2440,7 +2427,7 @@
       <c r="G52" s="51"/>
       <c r="H52" s="59"/>
     </row>
-    <row r="53" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>69</v>
       </c>
@@ -2453,25 +2440,22 @@
       <c r="D53" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E53" s="70" t="s">
-        <v>79</v>
+      <c r="E53" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F53" s="33" t="s">
         <v>79</v>
       </c>
       <c r="G53" s="50" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="J53" t="s">
-        <v>118</v>
-      </c>
-      <c r="K53" s="73"/>
-    </row>
-    <row r="54" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="J53" s="73"/>
+    </row>
+    <row r="54" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>70</v>
       </c>
@@ -2484,19 +2468,22 @@
       <c r="D54" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E54" s="70" t="s">
-        <v>79</v>
+      <c r="E54" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F54" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G54" s="49"/>
+      <c r="G54" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H54" s="8"/>
-      <c r="I54" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I54" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="J54" s="73"/>
+    </row>
+    <row r="55" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>25</v>
       </c>
@@ -2515,17 +2502,16 @@
       <c r="F55" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G55" s="49"/>
+      <c r="G55" s="49" t="s">
+        <v>118</v>
+      </c>
       <c r="H55" s="8"/>
       <c r="I55" s="68" t="s">
-        <v>125</v>
-      </c>
-      <c r="J55" t="s">
-        <v>118</v>
-      </c>
-      <c r="K55" s="67"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="J55" s="67"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>72</v>
       </c>
@@ -2552,7 +2538,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>73</v>
       </c>
@@ -2576,7 +2562,7 @@
       </c>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>74</v>
       </c>
@@ -2598,7 +2584,7 @@
       <c r="G58" s="49"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>75</v>
       </c>
@@ -2622,7 +2608,7 @@
       </c>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>112</v>
       </c>
@@ -2648,7 +2634,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>76</v>
       </c>
@@ -2670,7 +2656,7 @@
       <c r="G61" s="49"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>77</v>
       </c>
@@ -2694,7 +2680,7 @@
       </c>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>27</v>
       </c>
@@ -2716,7 +2702,7 @@
       <c r="G63" s="49"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>0</v>
       </c>
@@ -2738,7 +2724,7 @@
       <c r="G64" s="49"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>1</v>
       </c>
@@ -2760,7 +2746,7 @@
       <c r="G65" s="49"/>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>32</v>
       </c>
@@ -2782,7 +2768,7 @@
       <c r="G66" s="49"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>3</v>
       </c>
@@ -2804,7 +2790,7 @@
       <c r="G67" s="49"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:16380" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16379" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>4</v>
       </c>
@@ -2826,7 +2812,7 @@
       <c r="G68" s="25"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>5</v>
       </c>
@@ -2848,7 +2834,7 @@
       <c r="G69" s="49"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>6</v>
       </c>
@@ -2870,7 +2856,7 @@
       <c r="G70" s="49"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -2892,7 +2878,7 @@
       <c r="G71" s="49"/>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" spans="1:16380" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>9</v>
       </c>
@@ -2914,7 +2900,7 @@
       <c r="G72" s="49"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:16380" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>37</v>
       </c>
@@ -2936,7 +2922,7 @@
       <c r="G73" s="49"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +2944,7 @@
       <c r="G74" s="49"/>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>38</v>
       </c>
@@ -2980,7 +2966,7 @@
       <c r="G75" s="49"/>
       <c r="H75" s="8"/>
     </row>
-    <row r="76" spans="1:16380" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16379" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>40</v>
       </c>
@@ -19374,9 +19360,8 @@
       <c r="XEW76"/>
       <c r="XEX76"/>
       <c r="XEY76"/>
-      <c r="XEZ76"/>
-    </row>
-    <row r="77" spans="1:16380" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>106</v>
       </c>
@@ -19402,7 +19387,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:16380" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>12</v>
       </c>
@@ -19424,7 +19409,7 @@
       <c r="G78" s="49"/>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="1:16380" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>45</v>
       </c>
@@ -19446,7 +19431,7 @@
       <c r="G79" s="49"/>
       <c r="H79" s="8"/>
     </row>
-    <row r="80" spans="1:16380" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Tests Unitaires. Mise à jour 17Jan
Mise à Jour des descriptions dans le fichier de l'inventaire.
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -572,7 +572,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,31 +604,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -733,7 +715,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -901,27 +883,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1210,26 +1188,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:XEY240"/>
+  <dimension ref="A1:XEX240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="103" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21" style="31" customWidth="1"/>
+    <col min="6" max="6" width="21" style="31" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" style="54" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>101</v>
       </c>
@@ -1258,7 +1236,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>80</v>
       </c>
@@ -1278,7 +1256,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>81</v>
       </c>
@@ -1298,7 +1276,7 @@
       <c r="G3" s="30"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
@@ -1318,7 +1296,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>83</v>
       </c>
@@ -1338,7 +1316,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>84</v>
       </c>
@@ -1358,7 +1336,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>85</v>
       </c>
@@ -1378,7 +1356,7 @@
       <c r="G7" s="30"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>86</v>
       </c>
@@ -1398,7 +1376,7 @@
       <c r="G8" s="30"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>87</v>
       </c>
@@ -1418,7 +1396,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -1438,7 +1416,7 @@
       <c r="G10" s="30"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>89</v>
       </c>
@@ -1458,7 +1436,7 @@
       <c r="G11" s="30"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>90</v>
       </c>
@@ -1478,7 +1456,7 @@
       <c r="G12" s="30"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1500,7 +1478,7 @@
       <c r="G13" s="30"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
@@ -1522,7 +1500,7 @@
       <c r="G14" s="30"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>30</v>
       </c>
@@ -1535,7 +1513,7 @@
       <c r="D15" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="67" t="s">
         <v>79</v>
       </c>
       <c r="F15" s="33" t="s">
@@ -1547,7 +1525,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
@@ -1570,9 +1548,8 @@
         <v>130</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="J16" s="63"/>
-    </row>
-    <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>2</v>
       </c>
@@ -1594,7 +1571,7 @@
       <c r="G17" s="49"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
@@ -1616,7 +1593,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1639,12 +1616,11 @@
         <v>131</v>
       </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="68" t="s">
+      <c r="I19" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="J19" s="67"/>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -1653,12 +1629,11 @@
       <c r="F20" s="33"/>
       <c r="G20" s="49"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="68" t="s">
+      <c r="I20" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="J20" s="67"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1681,9 +1656,8 @@
         <v>118</v>
       </c>
       <c r="H21" s="8"/>
-      <c r="J21" s="63"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1705,7 +1679,7 @@
       <c r="G22" s="49"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>36</v>
       </c>
@@ -1718,7 +1692,7 @@
       <c r="D23" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="70" t="s">
+      <c r="E23" s="67" t="s">
         <v>79</v>
       </c>
       <c r="F23" s="33" t="s">
@@ -1732,7 +1706,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>111</v>
       </c>
@@ -1756,9 +1730,8 @@
       </c>
       <c r="H24" s="56"/>
       <c r="I24" s="60"/>
-      <c r="J24" s="65"/>
-    </row>
-    <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>39</v>
       </c>
@@ -1781,9 +1754,8 @@
         <v>118</v>
       </c>
       <c r="H25" s="8"/>
-      <c r="J25" s="63"/>
-    </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
@@ -1809,9 +1781,8 @@
       <c r="I26" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="J26" s="63"/>
-    </row>
-    <row r="27" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>42</v>
       </c>
@@ -1834,9 +1805,8 @@
         <v>118</v>
       </c>
       <c r="H27" s="8"/>
-      <c r="J27" s="66"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
@@ -1863,7 +1833,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
@@ -1886,9 +1856,8 @@
         <v>118</v>
       </c>
       <c r="H29" s="8"/>
-      <c r="J29" s="66"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>44</v>
       </c>
@@ -1911,9 +1880,8 @@
         <v>118</v>
       </c>
       <c r="H30" s="8"/>
-      <c r="J30" s="66"/>
-    </row>
-    <row r="31" spans="1:10" ht="33" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>47</v>
       </c>
@@ -1926,7 +1894,7 @@
       <c r="D31" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E31" s="71" t="s">
+      <c r="E31" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F31" s="33" t="s">
@@ -1940,7 +1908,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>48</v>
       </c>
@@ -1953,7 +1921,7 @@
       <c r="D32" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="71" t="s">
+      <c r="E32" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F32" s="33" t="s">
@@ -1962,7 +1930,7 @@
       <c r="G32" s="51"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>49</v>
       </c>
@@ -1975,7 +1943,7 @@
       <c r="D33" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="71" t="s">
+      <c r="E33" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F33" s="33" t="s">
@@ -1989,7 +1957,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>50</v>
       </c>
@@ -2002,7 +1970,7 @@
       <c r="D34" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="70" t="s">
+      <c r="E34" s="67" t="s">
         <v>79</v>
       </c>
       <c r="F34" s="33" t="s">
@@ -2016,7 +1984,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>114</v>
       </c>
@@ -2042,7 +2010,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>51</v>
       </c>
@@ -2055,7 +2023,7 @@
       <c r="D36" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="71" t="s">
+      <c r="E36" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F36" s="33" t="s">
@@ -2064,7 +2032,7 @@
       <c r="G36" s="51"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>52</v>
       </c>
@@ -2077,7 +2045,7 @@
       <c r="D37" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="71" t="s">
+      <c r="E37" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F37" s="33" t="s">
@@ -2086,7 +2054,7 @@
       <c r="G37" s="51"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
@@ -2108,7 +2076,7 @@
       <c r="G38" s="49"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:10" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>54</v>
       </c>
@@ -2130,7 +2098,7 @@
       <c r="G39" s="49"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>55</v>
       </c>
@@ -2152,7 +2120,7 @@
       <c r="G40" s="25"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>14</v>
       </c>
@@ -2174,7 +2142,7 @@
       <c r="G41" s="49"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>57</v>
       </c>
@@ -2187,7 +2155,7 @@
       <c r="D42" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="72" t="s">
+      <c r="E42" s="69" t="s">
         <v>79</v>
       </c>
       <c r="F42" s="33" t="s">
@@ -2196,7 +2164,7 @@
       <c r="G42" s="49"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:10" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>61</v>
       </c>
@@ -2218,7 +2186,7 @@
       <c r="G43" s="25"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>62</v>
       </c>
@@ -2240,7 +2208,7 @@
       <c r="G44" s="49"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
@@ -2262,7 +2230,7 @@
       <c r="G45" s="49"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>64</v>
       </c>
@@ -2284,7 +2252,7 @@
       <c r="G46" s="49"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2274,7 @@
       <c r="G47" s="25"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>65</v>
       </c>
@@ -2332,9 +2300,8 @@
       <c r="I48" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="J48" s="67"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>21</v>
       </c>
@@ -2347,7 +2314,7 @@
       <c r="D49" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="71" t="s">
+      <c r="E49" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F49" s="33" t="s">
@@ -2361,7 +2328,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>66</v>
       </c>
@@ -2383,7 +2350,7 @@
       <c r="G50" s="49"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -2405,7 +2372,7 @@
       <c r="G51" s="49"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:10" s="22" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="22" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>67</v>
       </c>
@@ -2418,7 +2385,7 @@
       <c r="D52" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="71" t="s">
+      <c r="E52" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F52" s="58" t="s">
@@ -2427,7 +2394,7 @@
       <c r="G52" s="51"/>
       <c r="H52" s="59"/>
     </row>
-    <row r="53" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>69</v>
       </c>
@@ -2450,12 +2417,11 @@
         <v>130</v>
       </c>
       <c r="H53" s="8"/>
-      <c r="I53" s="69" t="s">
+      <c r="I53" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="J53" s="73"/>
-    </row>
-    <row r="54" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>70</v>
       </c>
@@ -2478,12 +2444,11 @@
         <v>118</v>
       </c>
       <c r="H54" s="8"/>
-      <c r="I54" s="69" t="s">
+      <c r="I54" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="J54" s="73"/>
-    </row>
-    <row r="55" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>25</v>
       </c>
@@ -2506,12 +2471,11 @@
         <v>118</v>
       </c>
       <c r="H55" s="8"/>
-      <c r="I55" s="68" t="s">
+      <c r="I55" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="J55" s="67"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>72</v>
       </c>
@@ -2524,7 +2488,7 @@
       <c r="D56" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E56" s="71" t="s">
+      <c r="E56" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F56" s="33" t="s">
@@ -2538,7 +2502,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>73</v>
       </c>
@@ -2562,7 +2526,7 @@
       </c>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>74</v>
       </c>
@@ -2575,7 +2539,7 @@
       <c r="D58" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E58" s="71" t="s">
+      <c r="E58" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F58" s="33" t="s">
@@ -2584,7 +2548,7 @@
       <c r="G58" s="49"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>75</v>
       </c>
@@ -2608,7 +2572,7 @@
       </c>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>112</v>
       </c>
@@ -2634,7 +2598,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>76</v>
       </c>
@@ -2647,7 +2611,7 @@
       <c r="D61" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="71" t="s">
+      <c r="E61" s="68" t="s">
         <v>79</v>
       </c>
       <c r="F61" s="33" t="s">
@@ -2656,7 +2620,7 @@
       <c r="G61" s="49"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>77</v>
       </c>
@@ -2680,7 +2644,7 @@
       </c>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>27</v>
       </c>
@@ -2702,7 +2666,7 @@
       <c r="G63" s="49"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>0</v>
       </c>
@@ -2724,7 +2688,7 @@
       <c r="G64" s="49"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>1</v>
       </c>
@@ -2746,7 +2710,7 @@
       <c r="G65" s="49"/>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>32</v>
       </c>
@@ -2768,7 +2732,7 @@
       <c r="G66" s="49"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>3</v>
       </c>
@@ -2790,7 +2754,7 @@
       <c r="G67" s="49"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:16379" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16378" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>4</v>
       </c>
@@ -2812,7 +2776,7 @@
       <c r="G68" s="25"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>5</v>
       </c>
@@ -2834,7 +2798,7 @@
       <c r="G69" s="49"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>6</v>
       </c>
@@ -2856,7 +2820,7 @@
       <c r="G70" s="49"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -2878,7 +2842,7 @@
       <c r="G71" s="49"/>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16378" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>9</v>
       </c>
@@ -2900,7 +2864,7 @@
       <c r="G72" s="49"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16378" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>37</v>
       </c>
@@ -2922,7 +2886,7 @@
       <c r="G73" s="49"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>10</v>
       </c>
@@ -2944,7 +2908,7 @@
       <c r="G74" s="49"/>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>38</v>
       </c>
@@ -2966,7 +2930,7 @@
       <c r="G75" s="49"/>
       <c r="H75" s="8"/>
     </row>
-    <row r="76" spans="1:16379" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16378" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>40</v>
       </c>
@@ -19359,9 +19323,8 @@
       <c r="XEV76"/>
       <c r="XEW76"/>
       <c r="XEX76"/>
-      <c r="XEY76"/>
-    </row>
-    <row r="77" spans="1:16379" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>106</v>
       </c>
@@ -19387,7 +19350,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16378" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>12</v>
       </c>
@@ -19409,7 +19372,7 @@
       <c r="G78" s="49"/>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="1:16379" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16378" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>45</v>
       </c>
@@ -19431,7 +19394,7 @@
       <c r="G79" s="49"/>
       <c r="H79" s="8"/>
     </row>
-    <row r="80" spans="1:16379" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16378" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
ajustement des fichiers TestUnitaires
petits modification aux fichiers de relation des tests unitaires.
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$176</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$174</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="159">
   <si>
     <t>AB_MISSING_ATTRIBUTE_MANAGER</t>
   </si>
@@ -498,12 +498,6 @@
     <t>Autres Unit Tests dans le repertoire</t>
   </si>
   <si>
-    <t>Fgeoport</t>
-  </si>
-  <si>
-    <t>GEO_NONE_GEO_SELECTOR.fmx</t>
-  </si>
-  <si>
     <t>Inexistent Attribute in 'etalon' files
   --  xlsx_type:xlsx_none
  Inexistent attributes in 'results' file
@@ -511,9 +505,6 @@
   </si>
   <si>
     <t>TO follow</t>
-  </si>
-  <si>
-    <t>QC_ATTRIBUTE_MAPPER.fmx</t>
   </si>
   <si>
     <t>Plusieurs attributes inexistents dans 'etalon':
@@ -526,6 +517,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>GEO_NONE_GEO_SELECTOR</t>
   </si>
 </sst>
 </file>
@@ -1301,10 +1295,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:XEX176"/>
+  <dimension ref="A1:XEX174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="103" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,7 +1818,7 @@
     </row>
     <row r="24" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>78</v>
@@ -2277,10 +2271,10 @@
       <c r="G41" s="48"/>
       <c r="H41" s="8"/>
       <c r="I41" s="61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J41" s="71" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2377,7 +2371,7 @@
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="65" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2529,7 +2523,7 @@
       </c>
       <c r="H51" s="8"/>
       <c r="I51" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="21" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
@@ -19922,7 +19916,7 @@
       <c r="G95" s="48"/>
       <c r="H95" s="8"/>
       <c r="I95" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19991,35 +19985,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A102" s="59" t="s">
-        <v>154</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C102" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G102" s="53" t="s">
-        <v>117</v>
+        <v>143</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="E102" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A103" s="59" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B103" s="2"/>
-      <c r="E103" s="3">
-        <v>7</v>
+      <c r="E103" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="G103" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="I103" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A104" s="59" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B104" s="2"/>
       <c r="E104" s="66" t="s">
@@ -20029,360 +20021,333 @@
         <v>117</v>
       </c>
       <c r="I104" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="59" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B105" s="2"/>
-      <c r="E105" s="7" t="s">
-        <v>78</v>
+      <c r="E105" s="66" t="s">
+        <v>79</v>
       </c>
       <c r="G105" s="53" t="s">
         <v>117</v>
       </c>
+      <c r="I105" s="65" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="106" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="B106" s="2"/>
-      <c r="E106" s="66" t="s">
-        <v>79</v>
-      </c>
-      <c r="G106" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="I106" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="B106" s="1"/>
+      <c r="E106" s="3">
+        <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A107" s="59" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
       <c r="B107" s="2"/>
-      <c r="E107" s="66" t="s">
-        <v>79</v>
-      </c>
-      <c r="G107" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="I107" s="65" t="s">
-        <v>151</v>
+      <c r="E107" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="59" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="B108" s="1"/>
       <c r="E108" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="B109" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="B109" s="1"/>
       <c r="E109" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="59" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B110" s="1"/>
       <c r="E110" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="B111" s="1"/>
-      <c r="E111" s="3">
-        <v>4</v>
-      </c>
+    <row r="111" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B111" s="40"/>
+      <c r="C111" s="52"/>
+      <c r="E111"/>
+      <c r="F111"/>
+      <c r="G111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="59" t="s">
-        <v>90</v>
-      </c>
+      <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-      <c r="E112" s="3">
-        <v>5</v>
-      </c>
     </row>
-    <row r="113" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="B113" s="40"/>
-      <c r="C113" s="52"/>
-      <c r="E113"/>
-      <c r="F113"/>
-      <c r="G113"/>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
+    <row r="114" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="2"/>
-      <c r="B116" s="2"/>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
+    <row r="117" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
+    <row r="120" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
+    <row r="123" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
     </row>
-    <row r="125" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
+    <row r="126" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
     </row>
-    <row r="128" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
+    <row r="129" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
     </row>
-    <row r="131" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
+    <row r="132" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
     </row>
-    <row r="134" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
+    <row r="135" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
     </row>
-    <row r="137" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
+    <row r="138" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
-      <c r="B141" s="1"/>
+    <row r="141" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
+    <row r="144" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+      <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
     </row>
-    <row r="146" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
+    <row r="147" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
     </row>
-    <row r="149" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
+    <row r="150" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
     </row>
-    <row r="152" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A152" s="2"/>
-      <c r="B152" s="2"/>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
+    <row r="153" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
     </row>
-    <row r="155" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A155" s="2"/>
-      <c r="B155" s="2"/>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
+    <row r="156" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="2"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
     </row>
-    <row r="158" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A158" s="2"/>
-      <c r="B158" s="2"/>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
+    <row r="159" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A159" s="2"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
     </row>
-    <row r="161" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A161" s="2"/>
-      <c r="B161" s="2"/>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
+    <row r="162" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A162" s="2"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
     </row>
-    <row r="164" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A164" s="2"/>
-      <c r="B164" s="2"/>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
+    <row r="165" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A165" s="2"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
     </row>
-    <row r="167" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A167" s="2"/>
-      <c r="B167" s="2"/>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
+    <row r="168" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A168" s="2"/>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
     </row>
-    <row r="170" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A170" s="2"/>
-      <c r="B170" s="2"/>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
+    <row r="171" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2"/>
+      <c r="B171" s="2"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
     </row>
-    <row r="173" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A173" s="2"/>
-      <c r="B173" s="2"/>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
-    </row>
-    <row r="176" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A176" s="2"/>
-      <c r="B176" s="2"/>
+    <row r="174" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
+      <c r="B174" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H176">
+  <autoFilter ref="A1:H174">
     <filterColumn colId="3">
       <filters blank="1">
         <filter val="unitaire"/>

</xml_diff>

<commit_message>
Mise à jour DCAT_Reader
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DavidH\NRCan\fgp-metadata-proxy\FME_files\UNIT_TESTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FGP_GITHUB\fgp-metadata-proxy\FME_files\UNIT_TESTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="161">
   <si>
     <t>AB_MISSING_ATTRIBUTE_MANAGER</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>YT_CUSTOM_CATALOGUE_READER</t>
+  </si>
+  <si>
+    <t>A Besoin du serveur web fantoche (web_serveur)</t>
   </si>
 </sst>
 </file>
@@ -1473,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XEX166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="103" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1918,18 +1921,26 @@
       <c r="A19" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="66" t="s">
-        <v>79</v>
+      <c r="B19" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F19" s="31"/>
-      <c r="G19" s="43"/>
+      <c r="G19" s="43" t="s">
+        <v>98</v>
+      </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="59"/>
+      <c r="I19" s="59" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">

</xml_diff>

<commit_message>
Tests Untaires Mise à jour 25Jan22
Mise à jour de l'inventaire
Nouveau test pour NB_TAGS_MANAGER.
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FGP_GITHUB\fgp-metadata-proxy\FME_files\UNIT_TESTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DavidH\NRCan\Others\UNIT_TESTS-David_20Jan22\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$165</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="162">
   <si>
     <t>AB_MISSING_ATTRIBUTE_MANAGER</t>
   </si>
@@ -293,9 +293,6 @@
     <t>unitaire</t>
   </si>
   <si>
-    <t>processus</t>
-  </si>
-  <si>
     <t>Équivalent</t>
   </si>
   <si>
@@ -526,7 +523,13 @@
     <t>YT_CUSTOM_CATALOGUE_READER</t>
   </si>
   <si>
-    <t>A Besoin du serveur web fantoche (web_serveur)</t>
+    <t>Nombre des features differentes.</t>
+  </si>
+  <si>
+    <t>Non (Daniel)</t>
+  </si>
+  <si>
+    <t>OUi</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -722,6 +725,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,7 +824,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -916,25 +925,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -942,9 +935,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1006,13 +996,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1075,6 +1085,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1090,6 +1110,136 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1474,21 +1624,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XEX166"/>
+  <dimension ref="A1:XEX165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.7109375" style="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" style="27" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="48" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="41" customWidth="1"/>
     <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63.85546875" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -1496,7 +1646,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>85</v>
@@ -1505,22 +1655,22 @@
         <v>83</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>84</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1530,7 +1680,7 @@
       <c r="B2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -1543,38 +1693,37 @@
         <v>79</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="8"/>
+      <c r="I2" s="56" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="61" t="s">
-        <v>79</v>
+      <c r="B3" s="66" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="67" t="s">
+        <v>82</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="26"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="B4" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -1587,7 +1736,7 @@
         <v>79</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1598,7 +1747,7 @@
       <c r="B5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1610,19 +1759,19 @@
       <c r="F5" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="43" t="s">
-        <v>104</v>
+      <c r="G5" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="48" t="s">
+      <c r="B6" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -1634,8 +1783,8 @@
       <c r="F6" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="43" t="s">
-        <v>104</v>
+      <c r="G6" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H6" s="8"/>
     </row>
@@ -1646,13 +1795,13 @@
       <c r="B7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="65" t="s">
-        <v>134</v>
+      <c r="C7" s="58" t="s">
+        <v>133</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="67" t="s">
         <v>82</v>
       </c>
       <c r="F7" s="29" t="s">
@@ -1660,16 +1809,16 @@
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="57" t="s">
-        <v>107</v>
+      <c r="I7" s="50" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>78</v>
@@ -1683,44 +1832,41 @@
       <c r="F8" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="44" t="s">
-        <v>96</v>
+      <c r="G8" s="38" t="s">
+        <v>95</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="48" t="s">
+      <c r="A9" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="61" t="s">
-        <v>79</v>
+      <c r="E9" s="67" t="s">
+        <v>82</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="48" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
-        <v>137</v>
+      <c r="A10" s="47" t="s">
+        <v>136</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -1732,8 +1878,8 @@
       <c r="F10" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="43" t="s">
-        <v>104</v>
+      <c r="G10" s="37" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1743,7 +1889,7 @@
       <c r="B11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D11" s="15" t="s">
@@ -1755,8 +1901,8 @@
       <c r="F11" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="43" t="s">
-        <v>114</v>
+      <c r="G11" s="37" t="s">
+        <v>113</v>
       </c>
       <c r="H11" s="8"/>
     </row>
@@ -1767,7 +1913,7 @@
       <c r="B12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1777,58 +1923,52 @@
         <v>78</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="43"/>
+        <v>92</v>
+      </c>
+      <c r="G12" s="37"/>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="47" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>87</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="43" t="s">
-        <v>142</v>
+      <c r="G13" s="37" t="s">
+        <v>141</v>
       </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="57" t="s">
-        <v>145</v>
+      <c r="I13" s="56" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="43"/>
+      <c r="B14" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="58"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1838,7 +1978,7 @@
       <c r="B15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="15" t="s">
@@ -1850,17 +1990,17 @@
       <c r="F15" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="43"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="15" t="s">
@@ -1872,8 +2012,8 @@
       <c r="F16" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="48" t="s">
-        <v>104</v>
+      <c r="G16" s="41" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1883,7 +2023,7 @@
       <c r="B17" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D17" s="15" t="s">
@@ -1895,52 +2035,50 @@
       <c r="F17" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="43"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18" s="66" t="s">
+      <c r="A18" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
+      <c r="E18" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F18" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="43"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="59"/>
+      <c r="I18" s="52"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>78</v>
+      <c r="A19" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="67" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="67" t="s">
+        <v>82</v>
       </c>
       <c r="F19" s="31"/>
-      <c r="G19" s="43" t="s">
-        <v>98</v>
+      <c r="G19" s="37" t="s">
+        <v>97</v>
       </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="59" t="s">
-        <v>160</v>
-      </c>
+      <c r="I19" s="52"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -1961,7 +2099,7 @@
       <c r="F20" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="43"/>
+      <c r="G20" s="37"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1983,12 +2121,12 @@
       <c r="F21" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="43" t="s">
-        <v>115</v>
+      <c r="G21" s="37" t="s">
+        <v>114</v>
       </c>
       <c r="H21" s="8"/>
-      <c r="I21" s="59" t="s">
-        <v>132</v>
+      <c r="I21" s="52" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2010,11 +2148,11 @@
       <c r="F22" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G22" s="43"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="47" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -2032,14 +2170,14 @@
       <c r="F23" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="43" t="s">
-        <v>104</v>
+      <c r="G23" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="54" t="s">
-        <v>140</v>
+      <c r="A24" s="47" t="s">
+        <v>139</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>78</v>
@@ -2056,12 +2194,12 @@
       <c r="F24" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="48" t="s">
-        <v>104</v>
+      <c r="G24" s="41" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="47" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -2079,11 +2217,11 @@
       <c r="F25" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="43"/>
+      <c r="G25" s="37"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -2101,12 +2239,12 @@
       <c r="F26" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="43"/>
+      <c r="G26" s="37"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:9" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>78</v>
@@ -2124,13 +2262,13 @@
         <v>79</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" s="50"/>
-      <c r="I27" s="54"/>
+        <v>115</v>
+      </c>
+      <c r="H27" s="43"/>
+      <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="47" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -2146,10 +2284,10 @@
         <v>78</v>
       </c>
       <c r="F28" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2171,7 +2309,7 @@
       <c r="F29"/>
       <c r="G29"/>
       <c r="I29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2193,7 +2331,7 @@
       <c r="F30" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G30" s="43"/>
+      <c r="G30" s="37"/>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2215,7 +2353,7 @@
       <c r="F31" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G31" s="43"/>
+      <c r="G31" s="37"/>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2237,12 +2375,12 @@
       <c r="F32" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G32" s="43" t="s">
-        <v>104</v>
+      <c r="G32" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:16378" s="51" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16378" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>40</v>
       </c>
@@ -2263,7 +2401,7 @@
       </c>
       <c r="G33"/>
       <c r="H33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I33"/>
       <c r="J33"/>
@@ -18638,7 +18776,7 @@
     </row>
     <row r="34" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>78</v>
@@ -18655,8 +18793,8 @@
       <c r="F34" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="43" t="s">
-        <v>98</v>
+      <c r="G34" s="37" t="s">
+        <v>97</v>
       </c>
       <c r="H34" s="8"/>
     </row>
@@ -18679,12 +18817,12 @@
       <c r="F35" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="55" t="s">
+      <c r="G35" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="8"/>
+      <c r="I35" s="49" t="s">
         <v>104</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="56" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18706,12 +18844,12 @@
       <c r="F36" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G36" s="43" t="s">
-        <v>104</v>
+      <c r="G36" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18733,12 +18871,12 @@
       <c r="F37" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="43" t="s">
-        <v>104</v>
+      <c r="G37" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18760,12 +18898,12 @@
       <c r="F38" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G38" s="43" t="s">
-        <v>104</v>
+      <c r="G38" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18787,12 +18925,12 @@
       <c r="F39" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="43" t="s">
-        <v>104</v>
+      <c r="G39" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H39" s="8"/>
       <c r="I39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18814,7 +18952,7 @@
       <c r="F40" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G40" s="43"/>
+      <c r="G40" s="37"/>
       <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18825,7 +18963,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D41" s="16" t="s">
         <v>87</v>
@@ -18836,10 +18974,10 @@
       <c r="F41" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G41" s="43"/>
+      <c r="G41" s="37"/>
       <c r="H41" s="8"/>
       <c r="I41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18861,7 +18999,7 @@
       <c r="F42" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G42" s="43"/>
+      <c r="G42" s="37"/>
       <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18883,12 +19021,12 @@
       <c r="F43" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G43" s="43"/>
+      <c r="G43" s="37"/>
       <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="54" t="s">
-        <v>147</v>
+      <c r="A44" s="47" t="s">
+        <v>146</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>78</v>
@@ -18921,18 +19059,18 @@
       <c r="D45" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="62" t="s">
+      <c r="E45" s="55" t="s">
         <v>79</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G45" s="45"/>
+      <c r="G45" s="39"/>
       <c r="H45" t="s">
-        <v>152</v>
-      </c>
-      <c r="I45" s="58" t="s">
-        <v>108</v>
+        <v>151</v>
+      </c>
+      <c r="I45" s="51" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
@@ -18948,13 +19086,16 @@
       <c r="D46" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E46" s="62" t="s">
+      <c r="E46" s="55" t="s">
         <v>79</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G46" s="45"/>
+      <c r="G46" s="39"/>
+      <c r="I46" s="51" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="47" spans="1:16378" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
@@ -18969,23 +19110,23 @@
       <c r="D47" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E47" s="62" t="s">
+      <c r="E47" s="55" t="s">
         <v>79</v>
       </c>
       <c r="F47" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G47" s="43"/>
+      <c r="G47" s="37"/>
       <c r="H47" t="s">
-        <v>158</v>
-      </c>
-      <c r="I47" s="58" t="s">
-        <v>108</v>
+        <v>157</v>
+      </c>
+      <c r="I47" s="51" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:16378" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>78</v>
@@ -19002,8 +19143,8 @@
       <c r="F48" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="43" t="s">
-        <v>102</v>
+      <c r="G48" s="37" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19019,19 +19160,22 @@
       <c r="D49" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E49" s="61" t="s">
+      <c r="E49" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F49" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G49" s="43"/>
+      <c r="G49" s="37"/>
       <c r="H49" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="I49" s="51" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="67" t="s">
+      <c r="A50" s="60" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="18" t="s">
@@ -19043,14 +19187,17 @@
       <c r="D50" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E50" s="62" t="s">
+      <c r="E50" s="55" t="s">
         <v>79</v>
       </c>
       <c r="F50" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G50" s="45"/>
+      <c r="G50" s="37"/>
       <c r="H50" s="8"/>
+      <c r="I50" s="51" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="51" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
@@ -19065,21 +19212,24 @@
       <c r="D51" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E51" s="62" t="s">
+      <c r="E51" s="55" t="s">
         <v>79</v>
       </c>
       <c r="F51" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G51" s="45"/>
+      <c r="G51" s="37"/>
       <c r="H51" s="8"/>
+      <c r="I51" s="51" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="52" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="48" t="s">
-        <v>133</v>
+      <c r="B52" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>78</v>
@@ -19087,20 +19237,22 @@
       <c r="D52" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E52"/>
+      <c r="E52" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F52" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G52" t="s">
-        <v>142</v>
+      <c r="G52" s="37" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54" t="s">
-        <v>148</v>
-      </c>
-      <c r="B53" s="48" t="s">
-        <v>133</v>
+      <c r="A53" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>78</v>
@@ -19108,8 +19260,8 @@
       <c r="F53" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="G53" t="s">
-        <v>142</v>
+      <c r="G53" s="37" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19131,14 +19283,14 @@
       <c r="F54" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G54" s="43" t="s">
-        <v>104</v>
+      <c r="G54" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" t="s">
-        <v>118</v>
-      </c>
-      <c r="J54" s="63"/>
+        <v>117</v>
+      </c>
+      <c r="J54" s="56"/>
     </row>
     <row r="55" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -19159,12 +19311,12 @@
       <c r="F55" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G55" s="43"/>
+      <c r="G55" s="37"/>
       <c r="H55" s="8"/>
-      <c r="I55" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="J55" s="63"/>
+      <c r="I55" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="J55" s="56"/>
     </row>
     <row r="56" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
@@ -19185,11 +19337,11 @@
       <c r="F56" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="G56" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="I56" t="s">
-        <v>123</v>
+      <c r="G56" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="I56" s="56" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19211,7 +19363,7 @@
       <c r="F57" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G57" s="43"/>
+      <c r="G57" s="37"/>
       <c r="H57" s="8"/>
     </row>
     <row r="58" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19233,15 +19385,15 @@
       <c r="F58" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G58" s="43" t="s">
-        <v>142</v>
+      <c r="G58" s="37" t="s">
+        <v>141</v>
       </c>
       <c r="H58" s="8"/>
-      <c r="I58" s="56" t="s">
+      <c r="I58" s="68" t="s">
+        <v>125</v>
+      </c>
+      <c r="J58" s="57" t="s">
         <v>126</v>
-      </c>
-      <c r="J58" s="64" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19263,7 +19415,7 @@
       <c r="F59" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G59" s="43"/>
+      <c r="G59" s="37"/>
       <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19285,10 +19437,10 @@
       <c r="F60" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G60" s="43"/>
+      <c r="G60" s="37"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>59</v>
       </c>
@@ -19307,32 +19459,32 @@
       <c r="F61" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G61" s="43"/>
+      <c r="G61" s="37"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:10" s="14" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="36" t="s">
+    <row r="62" spans="1:10" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" s="40" t="s">
+      <c r="B62" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="16" t="s">
         <v>87</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F62" s="41" t="s">
+      <c r="F62" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G62" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="H62" s="42"/>
+      <c r="G62" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="H62" s="72"/>
     </row>
     <row r="63" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
@@ -19353,11 +19505,11 @@
       <c r="F63" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G63" s="43"/>
+      <c r="G63" s="37"/>
       <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="54" t="s">
+      <c r="A64" s="47" t="s">
         <v>61</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -19369,17 +19521,17 @@
       <c r="D64" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E64" s="61" t="s">
+      <c r="E64" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F64" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="G64" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="I64" t="s">
-        <v>124</v>
+      <c r="G64" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="I64" s="56" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19401,12 +19553,12 @@
       <c r="F65" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G65" s="43"/>
+      <c r="G65" s="37"/>
       <c r="H65" s="8"/>
       <c r="I65" t="s">
-        <v>120</v>
-      </c>
-      <c r="J65" s="63"/>
+        <v>119</v>
+      </c>
+      <c r="J65" s="56"/>
     </row>
     <row r="66" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
@@ -19427,12 +19579,12 @@
       <c r="F66" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G66" s="43" t="s">
-        <v>104</v>
+      <c r="G66" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H66" s="8"/>
-      <c r="I66" s="60" t="s">
-        <v>128</v>
+      <c r="I66" s="53" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19454,12 +19606,12 @@
       <c r="F67" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G67" s="43" t="s">
-        <v>104</v>
+      <c r="G67" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H67" s="8"/>
-      <c r="I67" s="56" t="s">
-        <v>109</v>
+      <c r="I67" s="49" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -19475,33 +19627,33 @@
       <c r="D68" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E68" s="61" t="s">
+      <c r="E68" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F68" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="G68" s="71" t="s">
-        <v>142</v>
+      <c r="G68" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H68" s="8"/>
-      <c r="I68" s="60" t="s">
-        <v>125</v>
+      <c r="I68" s="69" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="54" t="s">
-        <v>157</v>
-      </c>
-      <c r="B69" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="G69" s="71" t="s">
-        <v>142</v>
+      <c r="A69" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B69" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="G69" s="64" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="68" t="s">
+      <c r="A70" s="61" t="s">
         <v>18</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -19519,7 +19671,7 @@
       <c r="F70" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G70" s="43"/>
+      <c r="G70" s="37"/>
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19541,15 +19693,15 @@
       <c r="F71" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G71" s="43"/>
+      <c r="G71" s="37"/>
       <c r="H71" s="8"/>
     </row>
     <row r="72" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="54" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" s="48" t="s">
-        <v>133</v>
+      <c r="A72" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>82</v>
@@ -19561,17 +19713,17 @@
       <c r="F72" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G72" s="71" t="s">
-        <v>142</v>
+      <c r="G72" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H72" s="8"/>
     </row>
     <row r="73" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="B73" s="48" t="s">
-        <v>133</v>
+      <c r="A73" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>82</v>
@@ -19583,17 +19735,17 @@
       <c r="F73" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G73" s="71" t="s">
-        <v>142</v>
+      <c r="G73" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="54" t="s">
-        <v>150</v>
-      </c>
-      <c r="B74" s="48" t="s">
-        <v>133</v>
+      <c r="A74" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>82</v>
@@ -19605,17 +19757,17 @@
       <c r="F74" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G74" s="71" t="s">
-        <v>142</v>
+      <c r="G74" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H74" s="8"/>
     </row>
     <row r="75" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="54" t="s">
-        <v>151</v>
-      </c>
-      <c r="B75" s="48" t="s">
-        <v>133</v>
+      <c r="A75" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>82</v>
@@ -19625,19 +19777,19 @@
         <v>82</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="G75" s="71" t="s">
-        <v>142</v>
+        <v>93</v>
+      </c>
+      <c r="G75" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H75" s="8"/>
     </row>
     <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="54" t="s">
-        <v>152</v>
-      </c>
-      <c r="B76" s="48" t="s">
-        <v>133</v>
+      <c r="A76" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>82</v>
@@ -19649,17 +19801,17 @@
       <c r="F76" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G76" s="71" t="s">
-        <v>142</v>
+      <c r="G76" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="54" t="s">
-        <v>153</v>
-      </c>
-      <c r="B77" s="48" t="s">
-        <v>133</v>
+      <c r="A77" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>82</v>
@@ -19671,17 +19823,17 @@
       <c r="F77" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G77" s="71" t="s">
-        <v>142</v>
+      <c r="G77" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="B78" s="48" t="s">
-        <v>133</v>
+      <c r="A78" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>82</v>
@@ -19693,17 +19845,17 @@
       <c r="F78" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="G78" s="71" t="s">
-        <v>142</v>
+      <c r="G78" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H78" s="8"/>
     </row>
     <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79" s="48" t="s">
-        <v>133</v>
+      <c r="A79" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B79" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>82</v>
@@ -19715,8 +19867,8 @@
       <c r="F79" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G79" s="71" t="s">
-        <v>142</v>
+      <c r="G79" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H79" s="8"/>
     </row>
@@ -19737,15 +19889,15 @@
         <v>79</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="G80" s="71" t="s">
-        <v>142</v>
+        <v>93</v>
+      </c>
+      <c r="G80" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H80" s="8"/>
     </row>
-    <row r="81" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="67" t="s">
+    <row r="81" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="60" t="s">
         <v>20</v>
       </c>
       <c r="B81" s="18" t="s">
@@ -19763,12 +19915,12 @@
       <c r="F81" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G81" s="45"/>
+      <c r="G81" s="39"/>
       <c r="H81" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>22</v>
       </c>
@@ -19787,12 +19939,12 @@
       <c r="F82" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G82" s="45"/>
+      <c r="G82" s="39"/>
       <c r="H82" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>21</v>
       </c>
@@ -19805,21 +19957,21 @@
       <c r="D83" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E83" s="62" t="s">
+      <c r="E83" s="55" t="s">
         <v>79</v>
       </c>
       <c r="F83" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G83" s="45"/>
+      <c r="G83" s="39"/>
       <c r="H83" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="I83" s="58" t="s">
-        <v>108</v>
+        <v>146</v>
+      </c>
+      <c r="I83" s="51" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>65</v>
       </c>
@@ -19838,16 +19990,16 @@
       <c r="F84" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G84" s="43" t="s">
-        <v>104</v>
+      <c r="G84" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H84" s="8"/>
-      <c r="I84" s="56" t="s">
-        <v>109</v>
+      <c r="I84" s="49" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="68" t="s">
+    <row r="85" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="61" t="s">
         <v>66</v>
       </c>
       <c r="B85" s="5" t="s">
@@ -19865,10 +20017,10 @@
       <c r="F85" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G85" s="43"/>
+      <c r="G85" s="37"/>
       <c r="H85" s="8"/>
     </row>
-    <row r="86" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>23</v>
       </c>
@@ -19881,21 +20033,21 @@
       <c r="D86" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E86" s="61" t="s">
+      <c r="E86" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F86" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G86" s="43" t="s">
-        <v>104</v>
+      <c r="G86" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H86" s="8"/>
-      <c r="I86" t="s">
-        <v>129</v>
+      <c r="I86" s="56" t="s">
+        <v>128</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>24</v>
       </c>
@@ -19914,11 +20066,11 @@
       <c r="F87" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G87" s="43"/>
+      <c r="G87" s="37"/>
       <c r="H87" s="8"/>
     </row>
-    <row r="88" spans="1:9" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="67" t="s">
+    <row r="88" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="60" t="s">
         <v>67</v>
       </c>
       <c r="B88" s="18" t="s">
@@ -19930,16 +20082,16 @@
       <c r="D88" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E88" s="62" t="s">
+      <c r="E88" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="F88" s="52" t="s">
+      <c r="F88" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="G88" s="45"/>
-      <c r="H88" s="53"/>
+      <c r="G88" s="39"/>
+      <c r="H88" s="46"/>
     </row>
-    <row r="89" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>68</v>
       </c>
@@ -19958,10 +20110,10 @@
       <c r="F89" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G89" s="43"/>
+      <c r="G89" s="37"/>
       <c r="H89" s="8"/>
     </row>
-    <row r="90" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>69</v>
       </c>
@@ -19974,22 +20126,22 @@
       <c r="D90" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E90" s="61" t="s">
+      <c r="E90" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F90" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G90" s="43" t="s">
-        <v>114</v>
+      <c r="G90" s="37" t="s">
+        <v>113</v>
       </c>
       <c r="H90" s="8"/>
-      <c r="I90" s="60" t="s">
-        <v>112</v>
+      <c r="I90" s="69" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="68" t="s">
+    <row r="91" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="61" t="s">
         <v>70</v>
       </c>
       <c r="B91" s="5" t="s">
@@ -20005,17 +20157,17 @@
         <v>78</v>
       </c>
       <c r="F91" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="G91" s="43" t="s">
-        <v>104</v>
+        <v>92</v>
+      </c>
+      <c r="G91" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H91" s="8"/>
-      <c r="I91" s="60" t="s">
-        <v>113</v>
+      <c r="I91" s="53" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>71</v>
       </c>
@@ -20034,10 +20186,10 @@
       <c r="F92" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G92" s="43"/>
+      <c r="G92" s="37"/>
       <c r="H92" s="8"/>
     </row>
-    <row r="93" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>25</v>
       </c>
@@ -20056,16 +20208,16 @@
       <c r="F93" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G93" s="71" t="s">
-        <v>142</v>
+      <c r="G93" s="64" t="s">
+        <v>141</v>
       </c>
       <c r="H93" s="8"/>
-      <c r="I93" s="59" t="s">
-        <v>110</v>
+      <c r="I93" s="70" t="s">
+        <v>109</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="68" t="s">
+    <row r="94" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="61" t="s">
         <v>26</v>
       </c>
       <c r="B94" s="5" t="s">
@@ -20077,577 +20229,652 @@
       <c r="D94" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E94" s="61" t="s">
+      <c r="E94" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F94" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G94" s="43"/>
+      <c r="G94" s="37"/>
       <c r="H94" s="8"/>
       <c r="I94" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="29"/>
-      <c r="G95" s="43"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="59"/>
+    <row r="95" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E95" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G95" s="37"/>
+      <c r="H95" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I95" s="51" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="96" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B96" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C96" s="19" t="s">
-        <v>79</v>
+    <row r="96" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D96" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E96" s="62" t="s">
+      <c r="E96" s="9" t="s">
         <v>79</v>
       </c>
       <c r="F96" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G96" s="43"/>
-      <c r="H96" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="I96" s="58" t="s">
-        <v>108</v>
-      </c>
+      <c r="G96" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="H96" s="8"/>
+      <c r="I96" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="J96" s="56"/>
     </row>
-    <row r="97" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>73</v>
+    <row r="97" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D97" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G97" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="H97" s="8"/>
+    </row>
+    <row r="98" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C98" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D98" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E97" s="9" t="s">
+      <c r="E98" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="F97" s="29" t="s">
+      <c r="F98" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G97" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="H97" s="8"/>
-      <c r="I97" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="J97" s="63"/>
-    </row>
-    <row r="98" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="G98" s="71" t="s">
-        <v>142</v>
-      </c>
+      <c r="G98" s="37"/>
       <c r="H98" s="8"/>
     </row>
     <row r="99" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="B99" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C99" s="19" t="s">
-        <v>79</v>
+      <c r="A99" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D99" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E99" s="62" t="s">
-        <v>79</v>
+      <c r="E99" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F99" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G99" s="43"/>
+      <c r="G99" s="38" t="s">
+        <v>95</v>
+      </c>
       <c r="H99" s="8"/>
+      <c r="I99" t="s">
+        <v>121</v>
+      </c>
+      <c r="J99" s="56"/>
     </row>
     <row r="100" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>78</v>
+      <c r="A100" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C100" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="D100" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E100" s="7" t="s">
-        <v>78</v>
+      <c r="E100" s="55" t="s">
+        <v>79</v>
       </c>
       <c r="F100" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G100" s="44" t="s">
-        <v>96</v>
-      </c>
+      <c r="G100" s="37"/>
       <c r="H100" s="8"/>
-      <c r="I100" t="s">
-        <v>122</v>
-      </c>
-      <c r="J100" s="63"/>
     </row>
     <row r="101" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B101" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C101" s="19" t="s">
-        <v>79</v>
+      <c r="A101" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D101" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E101" s="62" t="s">
-        <v>79</v>
+      <c r="E101" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F101" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G101" s="43"/>
+      <c r="G101" s="38" t="s">
+        <v>95</v>
+      </c>
       <c r="H101" s="8"/>
+      <c r="I101" t="s">
+        <v>121</v>
+      </c>
+      <c r="J101" s="56"/>
     </row>
-    <row r="102" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="68" t="s">
-        <v>77</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F102" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G102" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="H102" s="8"/>
-      <c r="I102" t="s">
-        <v>122</v>
-      </c>
-      <c r="J102" s="63"/>
+    <row r="102" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B102" s="36"/>
+      <c r="C102" s="40"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
     </row>
-    <row r="103" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B103" s="37"/>
-      <c r="C103" s="47"/>
-      <c r="E103"/>
-      <c r="F103"/>
-      <c r="G103"/>
+    <row r="103" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="62"/>
+      <c r="B103" s="1"/>
     </row>
     <row r="104" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="69"/>
+      <c r="A104" s="62"/>
       <c r="B104" s="1"/>
     </row>
     <row r="105" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="69"/>
-      <c r="B105" s="1"/>
+      <c r="A105" s="63"/>
+      <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="70"/>
-      <c r="B106" s="2"/>
+      <c r="A106" s="62"/>
+      <c r="B106" s="1"/>
     </row>
     <row r="107" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="69"/>
+      <c r="A107" s="62"/>
       <c r="B107" s="1"/>
     </row>
     <row r="108" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="69"/>
-      <c r="B108" s="1"/>
+      <c r="A108" s="63"/>
+      <c r="B108" s="2"/>
     </row>
     <row r="109" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="70"/>
-      <c r="B109" s="2"/>
+      <c r="A109" s="62"/>
+      <c r="B109" s="1"/>
     </row>
     <row r="110" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="69"/>
+      <c r="A110" s="62"/>
       <c r="B110" s="1"/>
     </row>
     <row r="111" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="69"/>
-      <c r="B111" s="1"/>
+      <c r="A111" s="63"/>
+      <c r="B111" s="2"/>
     </row>
     <row r="112" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="70"/>
-      <c r="B112" s="2"/>
+      <c r="A112" s="62"/>
+      <c r="B112" s="1"/>
     </row>
     <row r="113" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="69"/>
+      <c r="A113" s="62"/>
       <c r="B113" s="1"/>
     </row>
     <row r="114" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="69"/>
-      <c r="B114" s="1"/>
+      <c r="A114" s="63"/>
+      <c r="B114" s="2"/>
     </row>
     <row r="115" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="70"/>
-      <c r="B115" s="2"/>
+      <c r="A115" s="62"/>
+      <c r="B115" s="1"/>
     </row>
     <row r="116" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="69"/>
+      <c r="A116" s="62"/>
       <c r="B116" s="1"/>
     </row>
     <row r="117" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="69"/>
-      <c r="B117" s="1"/>
+      <c r="A117" s="63"/>
+      <c r="B117" s="2"/>
     </row>
     <row r="118" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="70"/>
-      <c r="B118" s="2"/>
+      <c r="A118" s="62"/>
+      <c r="B118" s="1"/>
     </row>
     <row r="119" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="69"/>
+      <c r="A119" s="62"/>
       <c r="B119" s="1"/>
     </row>
     <row r="120" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="69"/>
-      <c r="B120" s="1"/>
+      <c r="A120" s="63"/>
+      <c r="B120" s="2"/>
     </row>
     <row r="121" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="70"/>
-      <c r="B121" s="2"/>
+      <c r="A121" s="62"/>
+      <c r="B121" s="1"/>
     </row>
     <row r="122" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="69"/>
+      <c r="A122" s="62"/>
       <c r="B122" s="1"/>
     </row>
     <row r="123" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="69"/>
-      <c r="B123" s="1"/>
+      <c r="A123" s="63"/>
+      <c r="B123" s="2"/>
     </row>
     <row r="124" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="70"/>
-      <c r="B124" s="2"/>
+      <c r="A124" s="62"/>
+      <c r="B124" s="1"/>
     </row>
     <row r="125" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="69"/>
+      <c r="A125" s="62"/>
       <c r="B125" s="1"/>
     </row>
     <row r="126" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="69"/>
-      <c r="B126" s="1"/>
+      <c r="A126" s="63"/>
+      <c r="B126" s="2"/>
     </row>
     <row r="127" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="70"/>
-      <c r="B127" s="2"/>
+      <c r="A127" s="62"/>
+      <c r="B127" s="1"/>
     </row>
     <row r="128" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="69"/>
+      <c r="A128" s="62"/>
       <c r="B128" s="1"/>
     </row>
     <row r="129" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="69"/>
-      <c r="B129" s="1"/>
+      <c r="A129" s="63"/>
+      <c r="B129" s="2"/>
     </row>
     <row r="130" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="70"/>
-      <c r="B130" s="2"/>
+      <c r="A130" s="62"/>
+      <c r="B130" s="1"/>
     </row>
     <row r="131" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="69"/>
+      <c r="A131" s="62"/>
       <c r="B131" s="1"/>
     </row>
     <row r="132" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="69"/>
-      <c r="B132" s="1"/>
+      <c r="A132" s="63"/>
+      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="70"/>
-      <c r="B133" s="2"/>
+      <c r="A133" s="62"/>
+      <c r="B133" s="1"/>
     </row>
     <row r="134" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="69"/>
+      <c r="A134" s="62"/>
       <c r="B134" s="1"/>
     </row>
     <row r="135" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="69"/>
-      <c r="B135" s="1"/>
+      <c r="A135" s="63"/>
+      <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="70"/>
-      <c r="B136" s="2"/>
+      <c r="A136" s="62"/>
+      <c r="B136" s="1"/>
     </row>
     <row r="137" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="69"/>
+      <c r="A137" s="62"/>
       <c r="B137" s="1"/>
     </row>
     <row r="138" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="69"/>
-      <c r="B138" s="1"/>
+      <c r="A138" s="63"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="70"/>
-      <c r="B139" s="2"/>
+      <c r="A139" s="62"/>
+      <c r="B139" s="1"/>
     </row>
     <row r="140" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="69"/>
+      <c r="A140" s="62"/>
       <c r="B140" s="1"/>
     </row>
     <row r="141" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="69"/>
-      <c r="B141" s="1"/>
+      <c r="A141" s="63"/>
+      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="70"/>
-      <c r="B142" s="2"/>
+      <c r="A142" s="62"/>
+      <c r="B142" s="1"/>
     </row>
     <row r="143" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="69"/>
+      <c r="A143" s="62"/>
       <c r="B143" s="1"/>
     </row>
     <row r="144" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="69"/>
-      <c r="B144" s="1"/>
+      <c r="A144" s="63"/>
+      <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="70"/>
-      <c r="B145" s="2"/>
+      <c r="A145" s="62"/>
+      <c r="B145" s="1"/>
     </row>
     <row r="146" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="69"/>
+      <c r="A146" s="62"/>
       <c r="B146" s="1"/>
     </row>
     <row r="147" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="69"/>
-      <c r="B147" s="1"/>
+      <c r="A147" s="63"/>
+      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="70"/>
-      <c r="B148" s="2"/>
+      <c r="A148" s="62"/>
+      <c r="B148" s="1"/>
     </row>
     <row r="149" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="69"/>
+      <c r="A149" s="62"/>
       <c r="B149" s="1"/>
     </row>
     <row r="150" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="69"/>
-      <c r="B150" s="1"/>
+      <c r="A150" s="63"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="70"/>
-      <c r="B151" s="2"/>
+      <c r="A151" s="62"/>
+      <c r="B151" s="1"/>
     </row>
     <row r="152" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="69"/>
+      <c r="A152" s="62"/>
       <c r="B152" s="1"/>
     </row>
     <row r="153" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="69"/>
-      <c r="B153" s="1"/>
+      <c r="A153" s="63"/>
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="70"/>
-      <c r="B154" s="2"/>
+      <c r="A154" s="62"/>
+      <c r="B154" s="1"/>
     </row>
     <row r="155" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="69"/>
+      <c r="A155" s="62"/>
       <c r="B155" s="1"/>
     </row>
     <row r="156" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="69"/>
-      <c r="B156" s="1"/>
+      <c r="A156" s="63"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="70"/>
-      <c r="B157" s="2"/>
+      <c r="A157" s="62"/>
+      <c r="B157" s="1"/>
     </row>
     <row r="158" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="69"/>
+      <c r="A158" s="62"/>
       <c r="B158" s="1"/>
     </row>
     <row r="159" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="69"/>
-      <c r="B159" s="1"/>
+      <c r="A159" s="63"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="70"/>
-      <c r="B160" s="2"/>
+      <c r="A160" s="62"/>
+      <c r="B160" s="1"/>
     </row>
     <row r="161" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="69"/>
+      <c r="A161" s="62"/>
       <c r="B161" s="1"/>
     </row>
     <row r="162" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="69"/>
-      <c r="B162" s="1"/>
+      <c r="A162" s="63"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="70"/>
-      <c r="B163" s="2"/>
+      <c r="A163" s="62"/>
+      <c r="B163" s="1"/>
     </row>
     <row r="164" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="69"/>
+      <c r="A164" s="62"/>
       <c r="B164" s="1"/>
     </row>
     <row r="165" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="69"/>
-      <c r="B165" s="1"/>
-    </row>
-    <row r="166" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="70"/>
-      <c r="B166" s="2"/>
+      <c r="A165" s="63"/>
+      <c r="B165" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4 B79">
-    <cfRule type="cellIs" dxfId="17" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="88" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 C15:C19">
-    <cfRule type="cellIs" dxfId="16" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="98" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 B79">
-    <cfRule type="expression" priority="62">
+    <cfRule type="expression" priority="89">
       <formula>isempty()</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="90" operator="equal">
       <formula>"'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="14" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="87" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="cellIs" dxfId="13" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="83" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" priority="54">
+    <cfRule type="expression" priority="81">
       <formula>isempty()</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="82" operator="equal">
       <formula>"'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="11" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="80" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="10" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="72" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C12">
-    <cfRule type="cellIs" dxfId="9" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="71" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="22" priority="64" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="expression" priority="35">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
+    <cfRule type="expression" priority="32">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="33" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
+    <cfRule type="cellIs" dxfId="18" priority="31" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B72:B78">
+    <cfRule type="expression" priority="29">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="30" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B72:B78">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="expression" priority="26">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="14" priority="25" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" priority="23">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="24" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="expression" priority="20">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="expression" priority="17">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" priority="14">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="expression" priority="11">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" priority="2">
+      <formula>isempty()</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" priority="39">
+    <cfRule type="expression" priority="5">
       <formula>isempty()</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="7" priority="38" operator="equal">
-      <formula>"n"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="6" priority="37" operator="equal">
-      <formula>"n"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="13">
-      <formula>IF($D$2="y",TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52:B53">
-    <cfRule type="expression" priority="8">
-      <formula>isempty()</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>"'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52:B53">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
-      <formula>"n"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
-    <cfRule type="expression" priority="5">
-      <formula>isempty()</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"n"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B72:B78">
-    <cfRule type="expression" priority="2">
-      <formula>isempty()</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B72:B78">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
New version of Spatial Data Validator
Major Refactoring
New Documentation
New Unit tests
Small documentation adjustement to SPATIAL_TYPE_MAPPER
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -1672,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XEX175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="103" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="103" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:XFD93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2440,7 +2440,7 @@
         <v>171</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>78</v>
@@ -2449,7 +2449,7 @@
         <v>87</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Mise à jour du fichier excel des tests unitaires
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
+++ b/FME_files/UNIT_TESTS/Inventaire_unit_test.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$180</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="198">
   <si>
     <t>AB_MISSING_ATTRIBUTE_MANAGER</t>
   </si>
@@ -626,6 +626,15 @@
   </si>
   <si>
     <t>Remplacer par METADATA_DELTA_FINDER_NG</t>
+  </si>
+  <si>
+    <t>NL_CATALOGUE_READER</t>
+  </si>
+  <si>
+    <t>NL_ATTRIBUTE_EXTRACTOR</t>
+  </si>
+  <si>
+    <t>A besoin de l'application WebServer.bat pour simuler un serveur web.</t>
   </si>
 </sst>
 </file>
@@ -1738,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XEX178"/>
+  <dimension ref="A1:XEX180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="103" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="103" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19309,7 +19318,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>12</v>
       </c>
@@ -19334,7 +19343,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>166</v>
       </c>
@@ -19361,7 +19370,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>45</v>
       </c>
@@ -19386,7 +19395,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>46</v>
       </c>
@@ -19408,7 +19417,7 @@
       <c r="G52" s="37"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>13</v>
       </c>
@@ -19430,9 +19439,9 @@
       <c r="G53" s="37"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="46" t="s">
-        <v>135</v>
+    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="67" t="s">
+        <v>196</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>78</v>
@@ -19449,63 +19458,63 @@
       <c r="F54" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G54" s="26"/>
+      <c r="G54" s="37" t="s">
+        <v>97</v>
+      </c>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>79</v>
+    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="67" t="s">
+        <v>195</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D55" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E55" s="54" t="s">
-        <v>79</v>
+      <c r="E55" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G55" s="39"/>
-      <c r="H55" t="s">
-        <v>139</v>
-      </c>
-      <c r="I55" s="50" t="s">
-        <v>107</v>
+        <v>78</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="H55" s="8"/>
+      <c r="I55" t="s">
+        <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>79</v>
+    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D56" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E56" s="54" t="s">
-        <v>79</v>
+      <c r="E56" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F56" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G56" s="39"/>
-      <c r="I56" s="50" t="s">
-        <v>107</v>
-      </c>
+      <c r="G56" s="26"/>
+      <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>78</v>
@@ -19522,40 +19531,41 @@
       <c r="F57" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G57" s="37"/>
+      <c r="G57" s="39"/>
       <c r="H57" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I57" s="50" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>78</v>
+    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="D58" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>78</v>
+      <c r="E58" s="54" t="s">
+        <v>79</v>
       </c>
       <c r="F58" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G58" s="37" t="s">
-        <v>101</v>
+      <c r="G58" s="39"/>
+      <c r="I58" s="50" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>78</v>
@@ -19566,7 +19576,7 @@
       <c r="D59" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="53" t="s">
+      <c r="E59" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F59" s="29" t="s">
@@ -19574,40 +19584,38 @@
       </c>
       <c r="G59" s="37"/>
       <c r="H59" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="I59" s="50" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>79</v>
+    <row r="60" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D60" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E60" s="54" t="s">
-        <v>79</v>
+      <c r="E60" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F60" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G60" s="37"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="50" t="s">
-        <v>107</v>
+      <c r="G60" s="37" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>78</v>
@@ -19618,67 +19626,73 @@
       <c r="D61" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E61" s="54" t="s">
+      <c r="E61" s="53" t="s">
         <v>79</v>
       </c>
       <c r="F61" s="29" t="s">
         <v>79</v>
       </c>
       <c r="G61" s="37"/>
-      <c r="H61" s="8"/>
+      <c r="H61" t="s">
+        <v>100</v>
+      </c>
       <c r="I61" s="50" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>78</v>
+    <row r="62" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="D62" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>78</v>
+      <c r="E62" s="54" t="s">
+        <v>79</v>
       </c>
       <c r="F62" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G62" s="37" t="s">
-        <v>103</v>
+      <c r="G62" s="37"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="50" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>78</v>
+    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="D63" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>78</v>
+      <c r="E63" s="54" t="s">
+        <v>79</v>
       </c>
       <c r="F63" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G63" s="37" t="s">
-        <v>103</v>
+      <c r="G63" s="37"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="50" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>53</v>
+    <row r="64" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>78</v>
@@ -19689,8 +19703,8 @@
       <c r="D64" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E64" s="9" t="s">
-        <v>79</v>
+      <c r="E64" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F64" s="29" t="s">
         <v>79</v>
@@ -19698,15 +19712,10 @@
       <c r="G64" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="H64" s="8"/>
-      <c r="I64" t="s">
-        <v>115</v>
-      </c>
-      <c r="J64" s="55"/>
     </row>
-    <row r="65" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>54</v>
+    <row r="65" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="46" t="s">
+        <v>136</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>78</v>
@@ -19723,14 +19732,13 @@
       <c r="F65" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G65" s="37"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="52"/>
-      <c r="J65" s="52"/>
+      <c r="G65" s="37" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="66" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>78</v>
@@ -19741,19 +19749,24 @@
       <c r="D66" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E66" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F66" s="31" t="s">
-        <v>78</v>
+      <c r="E66" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>79</v>
       </c>
       <c r="G66" s="37" t="s">
         <v>103</v>
       </c>
+      <c r="H66" s="8"/>
+      <c r="I66" t="s">
+        <v>115</v>
+      </c>
+      <c r="J66" s="55"/>
     </row>
-    <row r="67" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>78</v>
@@ -19772,10 +19785,12 @@
       </c>
       <c r="G67" s="37"/>
       <c r="H67" s="8"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="52"/>
     </row>
     <row r="68" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>78</v>
@@ -19789,42 +19804,38 @@
       <c r="E68" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F68" s="29" t="s">
-        <v>79</v>
+      <c r="F68" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="G68" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C69" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D69" s="34" t="s">
+    <row r="69" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E69" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="F69" s="44" t="s">
+      <c r="E69" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F69" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G69" s="39"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="20" t="s">
-        <v>183</v>
-      </c>
+      <c r="G69" s="37"/>
+      <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:10" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>78</v>
@@ -19839,40 +19850,41 @@
         <v>78</v>
       </c>
       <c r="F70" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="G70" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="I70" s="43" t="s">
-        <v>161</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G70" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D71" s="16" t="s">
+    <row r="71" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D71" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E71" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F71" s="29" t="s">
+      <c r="E71" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F71" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="G71" s="37"/>
-      <c r="H71" s="8"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="20" t="s">
+        <v>183</v>
+      </c>
     </row>
-    <row r="72" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>78</v>
@@ -19887,14 +19899,18 @@
         <v>78</v>
       </c>
       <c r="F72" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G72" s="37"/>
-      <c r="H72" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="G72" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="I72" s="43" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="73" spans="1:10" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="67" t="s">
-        <v>60</v>
+    <row r="73" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>78</v>
@@ -19911,15 +19927,12 @@
       <c r="F73" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G73" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="H73" s="68"/>
-      <c r="J73"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>78</v>
@@ -19939,9 +19952,9 @@
       <c r="G74" s="37"/>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="46" t="s">
-        <v>61</v>
+    <row r="75" spans="1:10" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="67" t="s">
+        <v>60</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>78</v>
@@ -19955,16 +19968,18 @@
       <c r="E75" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F75" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G75" s="41" t="s">
+      <c r="F75" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G75" s="37" t="s">
         <v>103</v>
       </c>
+      <c r="H75" s="68"/>
+      <c r="J75"/>
     </row>
     <row r="76" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>78</v>
@@ -19983,14 +19998,10 @@
       </c>
       <c r="G76" s="37"/>
       <c r="H76" s="8"/>
-      <c r="I76" t="s">
-        <v>116</v>
-      </c>
-      <c r="J76" s="55"/>
     </row>
     <row r="77" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>63</v>
+      <c r="A77" s="46" t="s">
+        <v>61</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>78</v>
@@ -20004,20 +20015,16 @@
       <c r="E77" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F77" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G77" s="37" t="s">
+      <c r="F77" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="G77" s="41" t="s">
         <v>103</v>
-      </c>
-      <c r="H77" s="8"/>
-      <c r="I77" s="52" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>78</v>
@@ -20034,17 +20041,16 @@
       <c r="F78" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G78" s="37" t="s">
-        <v>103</v>
-      </c>
+      <c r="G78" s="37"/>
       <c r="H78" s="8"/>
-      <c r="I78" s="48" t="s">
-        <v>108</v>
-      </c>
+      <c r="I78" t="s">
+        <v>116</v>
+      </c>
+      <c r="J78" s="55"/>
     </row>
-    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>78</v>
@@ -20055,40 +20061,50 @@
       <c r="D79" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E79" s="53" t="s">
+      <c r="E79" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F79" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="F79" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G79" s="62" t="s">
-        <v>131</v>
+      <c r="G79" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="H79" s="8"/>
-      <c r="I79" s="66" t="s">
-        <v>119</v>
+      <c r="I79" s="52" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="B80" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="C80" s="70" t="s">
-        <v>149</v>
-      </c>
-      <c r="G80" s="62" t="s">
+      <c r="A80" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F80" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G80" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="I80" s="71" t="s">
-        <v>148</v>
+      <c r="H80" s="8"/>
+      <c r="I80" s="48" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="59" t="s">
-        <v>18</v>
+    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>78</v>
@@ -20099,40 +20115,40 @@
       <c r="D81" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E81" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F81" s="29" t="s">
+      <c r="E81" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="G81" s="37"/>
+      <c r="F81" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="G81" s="62" t="s">
+        <v>131</v>
+      </c>
       <c r="H81" s="8"/>
+      <c r="I81" s="66" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="82" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D82" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F82" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G82" s="37"/>
-      <c r="H82" s="8"/>
+      <c r="A82" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C82" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="G82" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="I82" s="71" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="83" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="46" t="s">
-        <v>143</v>
+      <c r="A83" s="59" t="s">
+        <v>18</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>78</v>
@@ -20149,14 +20165,12 @@
       <c r="F83" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G83" s="62" t="s">
-        <v>103</v>
-      </c>
+      <c r="G83" s="37"/>
       <c r="H83" s="8"/>
     </row>
     <row r="84" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="46" t="s">
-        <v>137</v>
+      <c r="A84" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>78</v>
@@ -20173,14 +20187,12 @@
       <c r="F84" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G84" s="62" t="s">
-        <v>103</v>
-      </c>
+      <c r="G84" s="37"/>
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="46" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>78</v>
@@ -20204,7 +20216,7 @@
     </row>
     <row r="86" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>78</v>
@@ -20226,9 +20238,9 @@
       </c>
       <c r="H86" s="8"/>
     </row>
-    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="46" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>78</v>
@@ -20250,9 +20262,9 @@
       </c>
       <c r="H87" s="8"/>
     </row>
-    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="46" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>78</v>
@@ -20274,9 +20286,9 @@
       </c>
       <c r="H88" s="8"/>
     </row>
-    <row r="89" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="46" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>78</v>
@@ -20300,29 +20312,31 @@
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="B90" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F90" s="32" t="s">
-        <v>78</v>
+        <v>140</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F90" s="29" t="s">
+        <v>79</v>
       </c>
       <c r="G90" s="62" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="H90" s="8"/>
     </row>
     <row r="91" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>19</v>
+      <c r="A91" s="46" t="s">
+        <v>142</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>78</v>
@@ -20333,68 +20347,66 @@
       <c r="D91" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E91" s="9" t="s">
+      <c r="E91" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F91" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="F91" s="31" t="s">
-        <v>93</v>
-      </c>
       <c r="G91" s="62" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="H91" s="8"/>
     </row>
-    <row r="92" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="B92" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D92" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E92" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F92" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G92" s="39"/>
-      <c r="H92" s="22" t="s">
+    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="46" t="s">
         <v>141</v>
       </c>
+      <c r="B92" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F92" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G92" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="H92" s="8"/>
     </row>
     <row r="93" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B93" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>79</v>
+      <c r="A93" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D93" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E93" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F93" s="29" t="s">
+      <c r="E93" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G93" s="39"/>
-      <c r="H93" s="22" t="s">
-        <v>141</v>
-      </c>
+      <c r="F93" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="G93" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
-        <v>21</v>
+      <c r="A94" s="58" t="s">
+        <v>20</v>
       </c>
       <c r="B94" s="18" t="s">
         <v>78</v>
@@ -20405,98 +20417,98 @@
       <c r="D94" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E94" s="54" t="s">
-        <v>79</v>
+      <c r="E94" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="F94" s="29" t="s">
         <v>79</v>
       </c>
       <c r="G94" s="39"/>
-      <c r="H94" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="I94" s="50" t="s">
-        <v>107</v>
+      <c r="H94" s="22" t="s">
+        <v>141</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="B95" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C95" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D95" s="34" t="s">
+      <c r="C95" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D95" s="16" t="s">
         <v>87</v>
       </c>
       <c r="E95" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F95" s="44" t="s">
+      <c r="F95" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G95" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="H95" s="45"/>
-      <c r="I95" s="77" t="s">
-        <v>182</v>
+      <c r="G95" s="39"/>
+      <c r="H95" s="22" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>78</v>
+      <c r="A96" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="D96" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E96" s="7" t="s">
+      <c r="E96" s="54" t="s">
         <v>79</v>
       </c>
       <c r="F96" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G96" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="I96" s="8" t="s">
-        <v>181</v>
+      <c r="G96" s="39"/>
+      <c r="H96" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="I96" s="50" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D97" s="16" t="s">
+    <row r="97" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D97" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E97" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F97" s="29" t="s">
+      <c r="E97" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F97" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="G97" s="37"/>
-      <c r="H97" s="8"/>
+      <c r="G97" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="H97" s="45"/>
+      <c r="I97" s="77" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="98" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>78</v>
@@ -20507,23 +20519,22 @@
       <c r="D98" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E98" s="53" t="s">
+      <c r="E98" s="7" t="s">
         <v>79</v>
       </c>
       <c r="F98" s="29" t="s">
         <v>79</v>
       </c>
       <c r="G98" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="H98" s="8"/>
-      <c r="I98" s="55" t="s">
-        <v>121</v>
+        <v>97</v>
+      </c>
+      <c r="I98" s="8" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>24</v>
+      <c r="A99" s="59" t="s">
+        <v>66</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>78</v>
@@ -20543,31 +20554,36 @@
       <c r="G99" s="37"/>
       <c r="H99" s="8"/>
     </row>
-    <row r="100" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="B100" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C100" s="19" t="s">
+    <row r="100" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E100" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D100" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="E100" s="54" t="s">
+      <c r="F100" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="F100" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="G100" s="39"/>
-      <c r="H100" s="45"/>
+      <c r="G100" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="H100" s="8"/>
+      <c r="I100" s="55" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="101" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>78</v>
@@ -20587,36 +20603,31 @@
       <c r="G101" s="37"/>
       <c r="H101" s="8"/>
     </row>
-    <row r="102" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D102" s="16" t="s">
+    <row r="102" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C102" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D102" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E102" s="53" t="s">
+      <c r="E102" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="F102" s="29" t="s">
+      <c r="F102" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="G102" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="H102" s="8"/>
-      <c r="I102" s="66" t="s">
-        <v>109</v>
-      </c>
+      <c r="G102" s="39"/>
+      <c r="H102" s="45"/>
     </row>
     <row r="103" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="59" t="s">
-        <v>70</v>
+      <c r="A103" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>78</v>
@@ -20630,20 +20641,15 @@
       <c r="E103" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F103" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="G103" s="37" t="s">
-        <v>103</v>
-      </c>
+      <c r="F103" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G103" s="37"/>
       <c r="H103" s="8"/>
-      <c r="I103" s="52" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="104" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>78</v>
@@ -20654,18 +20660,23 @@
       <c r="D104" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E104" s="7" t="s">
-        <v>78</v>
+      <c r="E104" s="53" t="s">
+        <v>79</v>
       </c>
       <c r="F104" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G104" s="37"/>
+      <c r="G104" s="37" t="s">
+        <v>111</v>
+      </c>
       <c r="H104" s="8"/>
+      <c r="I104" s="66" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="105" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
-        <v>25</v>
+      <c r="A105" s="59" t="s">
+        <v>70</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>78</v>
@@ -20679,44 +20690,42 @@
       <c r="E105" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F105" s="29" t="s">
-        <v>79</v>
+      <c r="F105" s="31" t="s">
+        <v>92</v>
       </c>
       <c r="G105" s="37" t="s">
         <v>103</v>
       </c>
       <c r="H105" s="8"/>
+      <c r="I105" s="52" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="106" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="B106" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C106" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D106" s="34" t="s">
+    <row r="106" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D106" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E106" s="54" t="s">
+      <c r="E106" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F106" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="F106" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="G106" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="H106" s="45"/>
-      <c r="I106" s="20" t="s">
-        <v>191</v>
-      </c>
+      <c r="G106" s="37"/>
+      <c r="H106" s="8"/>
     </row>
     <row r="107" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="59" t="s">
-        <v>189</v>
+      <c r="A107" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>78</v>
@@ -20727,50 +20736,47 @@
       <c r="D107" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E107" s="53" t="s">
-        <v>79</v>
+      <c r="E107" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F107" s="29" t="s">
         <v>79</v>
       </c>
       <c r="G107" s="37" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H107" s="8"/>
-      <c r="I107" t="s">
-        <v>190</v>
-      </c>
     </row>
-    <row r="108" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="17" t="s">
-        <v>72</v>
+    <row r="108" spans="1:10" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="58" t="s">
+        <v>26</v>
       </c>
       <c r="B108" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C108" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D108" s="16" t="s">
+      <c r="C108" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D108" s="34" t="s">
         <v>87</v>
       </c>
       <c r="E108" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="F108" s="29" t="s">
+      <c r="F108" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="G108" s="37"/>
-      <c r="H108" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="I108" s="50" t="s">
-        <v>107</v>
+      <c r="G108" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="H108" s="45"/>
+      <c r="I108" s="20" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
-        <v>73</v>
+      <c r="A109" s="59" t="s">
+        <v>189</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>78</v>
@@ -20781,94 +20787,98 @@
       <c r="D109" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E109" s="9" t="s">
+      <c r="E109" s="53" t="s">
         <v>79</v>
       </c>
       <c r="F109" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G109" s="38" t="s">
-        <v>95</v>
+      <c r="G109" s="37" t="s">
+        <v>97</v>
       </c>
       <c r="H109" s="8"/>
-      <c r="I109" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="J109" s="55"/>
+      <c r="I109" t="s">
+        <v>190</v>
+      </c>
     </row>
-    <row r="110" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="B110" s="5" t="s">
+    <row r="110" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B110" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C110" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C110" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D110" s="10"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="G110" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="H110" s="8"/>
+      <c r="D110" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E110" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="F110" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G110" s="37"/>
+      <c r="H110" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I110" s="50" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="111" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B111" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C111" s="19" t="s">
-        <v>79</v>
+      <c r="A111" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D111" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E111" s="54" t="s">
+      <c r="E111" s="9" t="s">
         <v>79</v>
       </c>
       <c r="F111" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G111" s="37"/>
+      <c r="G111" s="38" t="s">
+        <v>95</v>
+      </c>
       <c r="H111" s="8"/>
+      <c r="I111" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="J111" s="55"/>
     </row>
-    <row r="112" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
-        <v>75</v>
+    <row r="112" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="46" t="s">
+        <v>81</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D112" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E112" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F112" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G112" s="38" t="s">
-        <v>95</v>
+      <c r="C112" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G112" s="62" t="s">
+        <v>131</v>
       </c>
       <c r="H112" s="8"/>
-      <c r="I112" t="s">
-        <v>118</v>
-      </c>
-      <c r="J112" s="55"/>
     </row>
     <row r="113" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="17" t="s">
-        <v>76</v>
+      <c r="A113" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="B113" s="18" t="s">
         <v>78</v>
@@ -20889,8 +20899,8 @@
       <c r="H113" s="8"/>
     </row>
     <row r="114" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="59" t="s">
-        <v>77</v>
+      <c r="A114" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>78</v>
@@ -20916,270 +20926,320 @@
       </c>
       <c r="J114" s="55"/>
     </row>
-    <row r="115" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B115" s="36"/>
-      <c r="C115" s="40"/>
-      <c r="E115"/>
-      <c r="F115"/>
-      <c r="G115"/>
+    <row r="115" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B115" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C115" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E115" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="F115" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G115" s="37"/>
+      <c r="H115" s="8"/>
     </row>
     <row r="116" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="60"/>
-      <c r="B116" s="1"/>
+      <c r="A116" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F116" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G116" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="H116" s="8"/>
+      <c r="I116" t="s">
+        <v>118</v>
+      </c>
+      <c r="J116" s="55"/>
     </row>
-    <row r="117" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="60"/>
-      <c r="B117" s="1"/>
+    <row r="117" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B117" s="36"/>
+      <c r="C117" s="40"/>
+      <c r="E117"/>
+      <c r="F117"/>
+      <c r="G117"/>
     </row>
     <row r="118" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="61"/>
-      <c r="B118" s="2"/>
+      <c r="A118" s="60"/>
+      <c r="B118" s="1"/>
     </row>
     <row r="119" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="60"/>
       <c r="B119" s="1"/>
     </row>
     <row r="120" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="60"/>
-      <c r="B120" s="1"/>
+      <c r="A120" s="61"/>
+      <c r="B120" s="2"/>
     </row>
     <row r="121" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="61"/>
-      <c r="B121" s="2"/>
+      <c r="A121" s="60"/>
+      <c r="B121" s="1"/>
     </row>
     <row r="122" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="60"/>
       <c r="B122" s="1"/>
     </row>
     <row r="123" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="60"/>
-      <c r="B123" s="1"/>
+      <c r="A123" s="61"/>
+      <c r="B123" s="2"/>
     </row>
     <row r="124" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="61"/>
-      <c r="B124" s="2"/>
+      <c r="A124" s="60"/>
+      <c r="B124" s="1"/>
     </row>
     <row r="125" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="60"/>
       <c r="B125" s="1"/>
     </row>
     <row r="126" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="60"/>
-      <c r="B126" s="1"/>
+      <c r="A126" s="61"/>
+      <c r="B126" s="2"/>
     </row>
     <row r="127" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="61"/>
-      <c r="B127" s="2"/>
+      <c r="A127" s="60"/>
+      <c r="B127" s="1"/>
     </row>
     <row r="128" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="60"/>
       <c r="B128" s="1"/>
     </row>
     <row r="129" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="60"/>
-      <c r="B129" s="1"/>
+      <c r="A129" s="61"/>
+      <c r="B129" s="2"/>
     </row>
     <row r="130" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="61"/>
-      <c r="B130" s="2"/>
+      <c r="A130" s="60"/>
+      <c r="B130" s="1"/>
     </row>
     <row r="131" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="60"/>
       <c r="B131" s="1"/>
     </row>
     <row r="132" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="60"/>
-      <c r="B132" s="1"/>
+      <c r="A132" s="61"/>
+      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="61"/>
-      <c r="B133" s="2"/>
+      <c r="A133" s="60"/>
+      <c r="B133" s="1"/>
     </row>
     <row r="134" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="60"/>
       <c r="B134" s="1"/>
     </row>
     <row r="135" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="60"/>
-      <c r="B135" s="1"/>
+      <c r="A135" s="61"/>
+      <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="61"/>
-      <c r="B136" s="2"/>
+      <c r="A136" s="60"/>
+      <c r="B136" s="1"/>
     </row>
     <row r="137" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="60"/>
       <c r="B137" s="1"/>
     </row>
     <row r="138" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="60"/>
-      <c r="B138" s="1"/>
+      <c r="A138" s="61"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="61"/>
-      <c r="B139" s="2"/>
+      <c r="A139" s="60"/>
+      <c r="B139" s="1"/>
     </row>
     <row r="140" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="60"/>
       <c r="B140" s="1"/>
     </row>
     <row r="141" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="60"/>
-      <c r="B141" s="1"/>
+      <c r="A141" s="61"/>
+      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="61"/>
-      <c r="B142" s="2"/>
+      <c r="A142" s="60"/>
+      <c r="B142" s="1"/>
     </row>
     <row r="143" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="60"/>
       <c r="B143" s="1"/>
     </row>
     <row r="144" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="60"/>
-      <c r="B144" s="1"/>
+      <c r="A144" s="61"/>
+      <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="61"/>
-      <c r="B145" s="2"/>
+      <c r="A145" s="60"/>
+      <c r="B145" s="1"/>
     </row>
     <row r="146" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="60"/>
       <c r="B146" s="1"/>
     </row>
     <row r="147" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="60"/>
-      <c r="B147" s="1"/>
+      <c r="A147" s="61"/>
+      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="61"/>
-      <c r="B148" s="2"/>
+      <c r="A148" s="60"/>
+      <c r="B148" s="1"/>
     </row>
     <row r="149" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="60"/>
       <c r="B149" s="1"/>
     </row>
     <row r="150" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="60"/>
-      <c r="B150" s="1"/>
+      <c r="A150" s="61"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="61"/>
-      <c r="B151" s="2"/>
+      <c r="A151" s="60"/>
+      <c r="B151" s="1"/>
     </row>
     <row r="152" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="60"/>
       <c r="B152" s="1"/>
     </row>
     <row r="153" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="60"/>
-      <c r="B153" s="1"/>
+      <c r="A153" s="61"/>
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="61"/>
-      <c r="B154" s="2"/>
+      <c r="A154" s="60"/>
+      <c r="B154" s="1"/>
     </row>
     <row r="155" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="60"/>
       <c r="B155" s="1"/>
     </row>
     <row r="156" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="60"/>
-      <c r="B156" s="1"/>
+      <c r="A156" s="61"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="61"/>
-      <c r="B157" s="2"/>
+      <c r="A157" s="60"/>
+      <c r="B157" s="1"/>
     </row>
     <row r="158" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="60"/>
       <c r="B158" s="1"/>
     </row>
     <row r="159" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="60"/>
-      <c r="B159" s="1"/>
+      <c r="A159" s="61"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="61"/>
-      <c r="B160" s="2"/>
+      <c r="A160" s="60"/>
+      <c r="B160" s="1"/>
     </row>
     <row r="161" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="60"/>
       <c r="B161" s="1"/>
     </row>
     <row r="162" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="60"/>
-      <c r="B162" s="1"/>
+      <c r="A162" s="61"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="61"/>
-      <c r="B163" s="2"/>
+      <c r="A163" s="60"/>
+      <c r="B163" s="1"/>
     </row>
     <row r="164" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="60"/>
       <c r="B164" s="1"/>
     </row>
     <row r="165" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="60"/>
-      <c r="B165" s="1"/>
+      <c r="A165" s="61"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="61"/>
-      <c r="B166" s="2"/>
+      <c r="A166" s="60"/>
+      <c r="B166" s="1"/>
     </row>
     <row r="167" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="60"/>
       <c r="B167" s="1"/>
     </row>
     <row r="168" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="60"/>
-      <c r="B168" s="1"/>
+      <c r="A168" s="61"/>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="61"/>
-      <c r="B169" s="2"/>
+      <c r="A169" s="60"/>
+      <c r="B169" s="1"/>
     </row>
     <row r="170" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="60"/>
       <c r="B170" s="1"/>
     </row>
     <row r="171" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="60"/>
-      <c r="B171" s="1"/>
+      <c r="A171" s="61"/>
+      <c r="B171" s="2"/>
     </row>
     <row r="172" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="61"/>
-      <c r="B172" s="2"/>
+      <c r="A172" s="60"/>
+      <c r="B172" s="1"/>
     </row>
     <row r="173" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="60"/>
       <c r="B173" s="1"/>
     </row>
     <row r="174" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="60"/>
-      <c r="B174" s="1"/>
+      <c r="A174" s="61"/>
+      <c r="B174" s="2"/>
     </row>
     <row r="175" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="61"/>
-      <c r="B175" s="2"/>
+      <c r="A175" s="60"/>
+      <c r="B175" s="1"/>
     </row>
     <row r="176" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="60"/>
       <c r="B176" s="1"/>
     </row>
     <row r="177" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="60"/>
-      <c r="B177" s="1"/>
+      <c r="A177" s="61"/>
+      <c r="B177" s="2"/>
     </row>
     <row r="178" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="61"/>
-      <c r="B178" s="2"/>
+      <c r="A178" s="60"/>
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="60"/>
+      <c r="B179" s="1"/>
+    </row>
+    <row r="180" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="61"/>
+      <c r="B180" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B90">
+  <conditionalFormatting sqref="B92">
     <cfRule type="cellIs" dxfId="30" priority="101" operator="equal">
       <formula>"n"</formula>
     </cfRule>
@@ -21189,7 +21249,7 @@
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90">
+  <conditionalFormatting sqref="B92">
     <cfRule type="expression" priority="102">
       <formula>isempty()</formula>
     </cfRule>
@@ -21230,7 +21290,7 @@
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B80">
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="45">
       <formula>isempty()</formula>
     </cfRule>
@@ -21238,7 +21298,7 @@
       <formula>"'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B80">
+  <conditionalFormatting sqref="B82">
     <cfRule type="cellIs" dxfId="20" priority="44" operator="equal">
       <formula>"n"</formula>
     </cfRule>

</xml_diff>